<commit_message>
Poprawki w wyliczaniu zmiennych czasowych
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="216">
   <si>
     <t>zmienna</t>
   </si>
@@ -282,52 +282,18 @@
     <t>GEZBAZYD</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Średnie miesięczne zarobki w powiecie zamieszkania absolwenta dla przepracowanych miesięcy danego okienka (etat/netat/samoz).
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>- W wypadku niejednoznacznego mapowania PNA na TERYT liczymy wartość dla PNA jako prostą średnią z powiatów-kandydatów.
+    <t>Średnie miesięczne zarobki w powiecie zamieszkania absolwenta dla przepracowanych miesięcy danego okienka (etat/netat/samoz).
+- W wypadku niejednoznacznego mapowania PNA na TERYT liczymy wartość dla PNA jako prostą średnią z powiatów-kandydatów.
 - W wypadku niejednoznacznego PNA dla danego okresu liczymy wartość dla okresu jako średnią z wartości PNA-kandydatów.</t>
-    </r>
   </si>
   <si>
     <t>GEZBAZYD_V2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Średnie miesięczne zarobki w powiecie zamieszkania absolwenta dla całego okienka.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>- W wypadku niejednoznacznego mapowania PNA na TERYT liczymy wartość dla PNA jako prostą średnią z powiatów-kandydatów.
+    <t>Średnie miesięczne zarobki w powiecie zamieszkania absolwenta dla całego okienka.
+- W wypadku niejednoznacznego mapowania PNA na TERYT liczymy wartość dla PNA jako prostą średnią z powiatów-kandydatów.
 - W wypadku niejednoznacznego PNA dla danego okresu liczymy wartość dla okresu jako średnią z wartości PNA-kandydatów.
 - W wypadku braku danych ZUS dla danego okresu zastępujemy wartością ogólnopolską.</t>
-    </r>
   </si>
   <si>
     <t>ZILORAZD</t>
@@ -379,25 +345,8 @@
     <t>EEM</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NEM / LEN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(NA dla 0/0)</t>
-    </r>
+    <t>NEM / LEN
+(NA dla 0/0)</t>
   </si>
   <si>
     <t>NEM, LEN</t>
@@ -406,25 +355,8 @@
     <t>EEMP</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NEM / NME
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(NA dla 0/0)</t>
-    </r>
+    <t>NEM / NME
+(NA dla 0/0)</t>
   </si>
   <si>
     <t>NEM, NME</t>
@@ -443,25 +375,8 @@
     <t>ENDN</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NNDN * 12 / LEN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(NA dla 0/0)</t>
-    </r>
+    <t>NNDN * 12 / LEN
+(NA dla 0/0)</t>
   </si>
   <si>
     <t>NDN, LEN</t>
@@ -480,25 +395,8 @@
     <t>EPRNDAWD</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NDN / NMN
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(NA dla 0/0)</t>
-    </r>
+    <t>NDN / NMN
+(NA dla 0/0)</t>
   </si>
   <si>
     <t>NDN, NMN</t>
@@ -507,25 +405,8 @@
     <t>EPRUDAWD</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>NDE / NME 
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>(NA dla 0/0)</t>
-    </r>
+    <t>NDE / NME 
+(NA dla 0/0)</t>
   </si>
   <si>
     <t>NDE, NME</t>
@@ -604,25 +485,8 @@
     <t>MIEJZAM</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Akademickość miejsca zamieszkania na koniec okienka (wyjątek - w momencie uzyskania dyplomu dla okienka obejmującego cały okres od uzyskania dyplomu)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>W wypadku niejednoznacznego mapowania PNA na powiaty lub wiele wpisów dla tego samego okresu wskazuje na różne powiaty, wtedy NA.</t>
-    </r>
+    <t>Akademickość miejsca zamieszkania na koniec okienka (wyjątek - w momencie uzyskania dyplomu dla okienka obejmującego cały okres od uzyskania dyplomu)
+W wypadku niejednoznacznego mapowania PNA na powiaty lub wiele wpisów dla tego samego okresu wskazuje na różne powiaty, wtedy NA.</t>
   </si>
   <si>
     <t>powiaty 264, 461, 463, 663, 1061, 1261, 1465, 1863, 2061, 2261, 2262, 2469, 2862, 3064, 3262</t>
@@ -631,26 +495,9 @@
     <t>MIEJZAM_V2</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Akademickość miejsca zamieszkania na koniec okienka (wyjątek - w momencie uzyskania dyplomu dla okienka obejmującego cały okres od uzyskania dyplomu)
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>W wypadku niejednoznacznego mapowania PNA na powiaty przyjmowana minimalna wartość spośród powiatów-kandydatów.
+    <t>Akademickość miejsca zamieszkania na koniec okienka (wyjątek - w momencie uzyskania dyplomu dla okienka obejmującego cały okres od uzyskania dyplomu)
+W wypadku niejednoznacznego mapowania PNA na powiaty przyjmowana minimalna wartość spośród powiatów-kandydatów.
 W wypadku gdy wiele różnych PNA dla danego okresu, wtedy najmniejsza wartość spośród wartości PNA-kandydatów.</t>
-    </r>
   </si>
   <si>
     <t>MNPRD</t>
@@ -732,88 +579,85 @@
     <t>stała</t>
   </si>
   <si>
-    <t>W którym miesiącu od miesiąca uzyskania dyplomu absolwent podjął zatrudnienie W ZAWODOWYCH SŁUŻBACH MUNDUROWYCH (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił pracy u tego samego pracodawcy)</t>
+    <t>Okres składkowy uzyskania pierwszej pracy w służbach mundurowych (mundur) minus miesiąc uzyskania dyplomu (czas do uzyskania pierwszej pracy w służbach mundurowych w miesiącach)
+Wartość 0 tylko gdy utrzymał pracę o tym samym charakterze u tego samego pracodawcy w kolejnym miesiącu.</t>
   </si>
   <si>
     <t>oblicz_zmienne_czasowe</t>
   </si>
   <si>
+    <t>baza, utrataEtatu</t>
+  </si>
+  <si>
     <t>CZASPRAW_V2</t>
   </si>
   <si>
-    <t>W którym miesiącu od miesiąca uzyskania dyplomu absolwent podjął zatrudnienie jako aplikant, sędzia, prokurator (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił pracy u tego samego pracodawcy)</t>
+    <t>Okres składkowy uzyskania pierwszej pracy jako aplikant/sędzia/prokurator (prawnik) minus miesiąc uzyskania dyplomu (czas do uzyskania pierwszej pracy jako aplikant/sędzia/prokurator w miesiącach)
+Wartość 0 tylko gdy utrzymał pracę o tym samym charakterze u tego samego pracodawcy w kolejnym miesiącu.</t>
   </si>
   <si>
     <t>CZASPRD_V2</t>
   </si>
   <si>
-    <t>W którym miesiącu od miesiąca uzyskania dyplomu absolwent podjął pracę (samozatrudnienie, etat lub nieetat) (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił pracy u tego samego pracodawcy)</t>
+    <t>Okres składkowy uzyskania pierwszej pracy (etat/netat/samoz) minus miesiąc uzyskania dyplomu (czas do uzyskania pierwszej pracy w miesiącach)
+Wartość 0 tylko gdy utrzymał pracę o tym samym charakterze u tego samego pracodawcy w kolejnym miesiącu</t>
   </si>
   <si>
     <t>CZASPRSD_V2</t>
   </si>
   <si>
-    <t>W którym miesiącu od miesiąca uzyskania dyplomu absolwent podjął SAMOZATRUDNIENIE (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił pracy u tego samego pracodawcy)</t>
+    <t>Okres składkowy podjęcia pierwszej pracy jako samozatrudniony (samoz) jako  minus miesiąc uzyskania dyplomu (czas do podejęcia pierwszej pracy jako samozatrudniony)
+Wartość 0 tylko gdy utrzymał pracę o tym samym charakterze u tego samego pracodawcy w kolejnym miesiącu.</t>
   </si>
   <si>
     <t>CZASPRUD_V2</t>
   </si>
   <si>
-    <t>W którym miesiącu od miesiąca uzyskania dyplomu absolwent podjął pracę NA UMOWĘ O PRACĘ (etat) (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił pracy u tego samego pracodawcy)</t>
+    <t>Okres składkowy podjęcia pierwszej pracy etatowej (etat) jako  minus miesiąc uzyskania dyplomu (czas do podejęcia pierwszej pracy etatowek)
+Wartość 0 tylko gdy utrzymał pracę o tym samym charakterze u tego samego pracodawcy w kolejnym miesiącu.</t>
   </si>
   <si>
     <t>CZASZATD_V2</t>
   </si>
   <si>
-    <t>W którym miesiącu od miesiąca uzyskania dyplomu absolwent podjął zatrudnienie (etat lub nieetat) (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił pracy u tego samego pracodawcy)</t>
+    <t>Okres składkowy podjęcia pierwszej pracy na etat lub netat  minus miesiąc uzyskania dyplomu (czas do podejęcia pierwszej pracy na etat/netat)
+Wartość 0 tylko gdy utrzymał pracę o tym samym charakterze u tego samego pracodawcy w kolejnym miesiącu.</t>
   </si>
   <si>
     <t>CZASMUN</t>
   </si>
   <si>
-    <t>Ile pełnych miesięcy od dyplomu minęło do czasu, aż podjął zatrudnienie W ZAWODOWYCH SŁUŻBACH MUNDUROWYCH (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił tej pracy)</t>
+    <t>max(0, CZASMUN_V2 – 1)</t>
   </si>
   <si>
     <t>CZASPRAW</t>
   </si>
   <si>
-    <t>Ile pełnych miesięcy od dyplomu minęło do czasu, aż podjął zatrudnienie jako aplikant, sędzia, prokurator (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił tej pracy)</t>
+    <t>max(0, CZAPRAW_V2 – 1)</t>
   </si>
   <si>
     <t>CZASPRD</t>
   </si>
   <si>
-    <t>Ile pełnych miesięcy od dyplomu minęło do czasu, aż podjął pracę (samozatrudnienie, etat lub nieetat) (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0</t>
+    <t>max(0, CZASPRD_V2 – 1)</t>
   </si>
   <si>
     <t>CZASPRSD</t>
   </si>
   <si>
-    <t>Ile pełnych miesięcy od dyplomu minęło do czasu, aż podjął SAMOZATRUDNIENIE (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił tej pracy)</t>
+    <t>max(0, CZASPRSD_V2 – 1)</t>
   </si>
   <si>
     <t>CZASPRUD</t>
   </si>
   <si>
-    <t>Ile pełnych miesięcy od dyplomu minęło do czasu, aż podjął pracę NA UMOWĘ O PRACĘ (etat) (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił tej pracy)</t>
+    <t>max(0, CZASPRUD_V2 – 1)</t>
   </si>
   <si>
     <t>CZASZATD</t>
   </si>
   <si>
-    <t>Ile pełnych miesięcy od dyplomu minęło do czasu, aż podjął zatrudnienie (etat lub nieetat) (do ostatniego miesiąca objętego obserwacją w ZUS)
-wartości od 0 (w tym samym miesiącu co miesiąc uzyskania dyplomu, jeśli w następnym miesiącu nie utracił tej pracy)</t>
+    <t>max(0, CZASZATD_V2 – 1)</t>
   </si>
   <si>
     <t>KONT</t>
@@ -885,13 +729,12 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -913,7 +756,6 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -921,23 +763,15 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -954,12 +788,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEEEEEE"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -1011,7 +839,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1048,11 +876,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1139,20 +963,22 @@
   </sheetPr>
   <dimension ref="A1:N65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A49" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C50" activeCellId="0" sqref="C50"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D58" activeCellId="0" sqref="D58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.6785714285714"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="25.4948979591837"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.2755102040816"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="24.1632653061224"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="49.1377551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.280612244898"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="25.1071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.3622448979592"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1374,7 +1200,7 @@
       <c r="B8" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="s">
+      <c r="C8" s="6" t="s">
         <v>36</v>
       </c>
       <c r="D8" s="6"/>
@@ -2646,13 +2472,13 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="10" t="s">
+      <c r="A49" s="9" t="s">
         <v>147</v>
       </c>
-      <c r="B49" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C49" s="10" t="s">
+      <c r="B49" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C49" s="9" t="s">
         <v>148</v>
       </c>
       <c r="D49" s="6" t="s">
@@ -2677,13 +2503,13 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="10" t="s">
+      <c r="A50" s="9" t="s">
         <v>150</v>
       </c>
-      <c r="B50" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="C50" s="10" t="s">
+      <c r="B50" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C50" s="9" t="s">
         <v>151</v>
       </c>
       <c r="D50" s="6" t="s">
@@ -2937,13 +2763,13 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="9" t="s">
         <v>169</v>
       </c>
-      <c r="B58" s="10" t="s">
+      <c r="B58" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C58" s="10" t="s">
+      <c r="C58" s="9" t="s">
         <v>171</v>
       </c>
       <c r="D58" s="6"/>
@@ -2951,7 +2777,7 @@
         <v>172</v>
       </c>
       <c r="F58" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G58" s="6"/>
       <c r="H58" s="6"/>
@@ -2966,21 +2792,21 @@
       </c>
     </row>
     <row r="59" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="10" t="s">
-        <v>173</v>
-      </c>
-      <c r="B59" s="10" t="s">
+      <c r="A59" s="9" t="s">
+        <v>174</v>
+      </c>
+      <c r="B59" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C59" s="10" t="s">
-        <v>174</v>
+      <c r="C59" s="9" t="s">
+        <v>175</v>
       </c>
       <c r="D59" s="6"/>
       <c r="E59" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F59" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G59" s="6"/>
       <c r="H59" s="6"/>
@@ -2995,21 +2821,21 @@
       </c>
     </row>
     <row r="60" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="B60" s="10" t="s">
+      <c r="A60" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="B60" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C60" s="10" t="s">
-        <v>176</v>
+      <c r="C60" s="9" t="s">
+        <v>177</v>
       </c>
       <c r="D60" s="6"/>
       <c r="E60" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F60" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G60" s="6"/>
       <c r="H60" s="6"/>
@@ -3023,22 +2849,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="10" t="s">
-        <v>177</v>
-      </c>
-      <c r="B61" s="10" t="s">
+    <row r="61" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B61" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C61" s="10" t="s">
-        <v>178</v>
+      <c r="C61" s="9" t="s">
+        <v>179</v>
       </c>
       <c r="D61" s="6"/>
       <c r="E61" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F61" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G61" s="6"/>
       <c r="H61" s="6"/>
@@ -3053,21 +2879,21 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="B62" s="10" t="s">
+      <c r="A62" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="B62" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C62" s="10" t="s">
-        <v>180</v>
+      <c r="C62" s="9" t="s">
+        <v>181</v>
       </c>
       <c r="D62" s="6"/>
       <c r="E62" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F62" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G62" s="6"/>
       <c r="H62" s="6"/>
@@ -3082,21 +2908,21 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="10" t="s">
-        <v>181</v>
-      </c>
-      <c r="B63" s="10" t="s">
+      <c r="A63" s="9" t="s">
+        <v>182</v>
+      </c>
+      <c r="B63" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C63" s="10" t="s">
-        <v>182</v>
+      <c r="C63" s="9" t="s">
+        <v>183</v>
       </c>
       <c r="D63" s="6"/>
       <c r="E63" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F63" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G63" s="6"/>
       <c r="H63" s="6"/>
@@ -3110,22 +2936,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="10" t="s">
-        <v>183</v>
-      </c>
-      <c r="B64" s="10" t="s">
+    <row r="64" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="9" t="s">
+        <v>184</v>
+      </c>
+      <c r="B64" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C64" s="10" t="s">
-        <v>184</v>
-      </c>
-      <c r="D64" s="6"/>
+      <c r="C64" s="9" t="s">
+        <v>185</v>
+      </c>
+      <c r="D64" s="6" t="s">
+        <v>169</v>
+      </c>
       <c r="E64" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F64" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G64" s="6"/>
       <c r="H64" s="6"/>
@@ -3136,25 +2964,27 @@
       <c r="M64" s="6"/>
       <c r="N64" s="8" t="n">
         <f aca="false">D64=""</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="10" t="s">
-        <v>185</v>
-      </c>
-      <c r="B65" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="9" t="s">
+        <v>186</v>
+      </c>
+      <c r="B65" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C65" s="10" t="s">
-        <v>186</v>
-      </c>
-      <c r="D65" s="6"/>
+      <c r="C65" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="D65" s="6" t="s">
+        <v>174</v>
+      </c>
       <c r="E65" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F65" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G65" s="6"/>
       <c r="H65" s="6"/>
@@ -3165,25 +2995,27 @@
       <c r="M65" s="6"/>
       <c r="N65" s="8" t="n">
         <f aca="false">D65=""</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="10" t="s">
-        <v>187</v>
-      </c>
-      <c r="B66" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="B66" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C66" s="10" t="s">
-        <v>188</v>
-      </c>
-      <c r="D66" s="6"/>
+      <c r="C66" s="9" t="s">
+        <v>189</v>
+      </c>
+      <c r="D66" s="6" t="s">
+        <v>176</v>
+      </c>
       <c r="E66" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F66" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G66" s="6"/>
       <c r="H66" s="6"/>
@@ -3194,25 +3026,27 @@
       <c r="M66" s="6"/>
       <c r="N66" s="8" t="n">
         <f aca="false">D66=""</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="10" t="s">
-        <v>189</v>
-      </c>
-      <c r="B67" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="B67" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C67" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="D67" s="6"/>
+      <c r="C67" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="D67" s="6" t="s">
+        <v>178</v>
+      </c>
       <c r="E67" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F67" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G67" s="6"/>
       <c r="H67" s="6"/>
@@ -3223,25 +3057,27 @@
       <c r="M67" s="6"/>
       <c r="N67" s="8" t="n">
         <f aca="false">D67=""</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A68" s="10" t="s">
-        <v>191</v>
-      </c>
-      <c r="B68" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="9" t="s">
+        <v>192</v>
+      </c>
+      <c r="B68" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C68" s="10" t="s">
-        <v>192</v>
-      </c>
-      <c r="D68" s="6"/>
+      <c r="C68" s="9" t="s">
+        <v>193</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>180</v>
+      </c>
       <c r="E68" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F68" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G68" s="6"/>
       <c r="H68" s="6"/>
@@ -3252,25 +3088,27 @@
       <c r="M68" s="6"/>
       <c r="N68" s="8" t="n">
         <f aca="false">D68=""</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A69" s="10" t="s">
-        <v>193</v>
-      </c>
-      <c r="B69" s="10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="B69" s="9" t="s">
         <v>170</v>
       </c>
-      <c r="C69" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="D69" s="6"/>
+      <c r="C69" s="9" t="s">
+        <v>195</v>
+      </c>
+      <c r="D69" s="6" t="s">
+        <v>182</v>
+      </c>
       <c r="E69" s="7" t="s">
         <v>172</v>
       </c>
       <c r="F69" s="7" t="s">
-        <v>15</v>
+        <v>173</v>
       </c>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
@@ -3281,68 +3119,68 @@
       <c r="M69" s="6"/>
       <c r="N69" s="8" t="n">
         <f aca="false">D69=""</f>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>170</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="D70" s="6"/>
       <c r="E70" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F70" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G70" s="6" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="H70" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I70" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J70" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K70" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L70" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M70" s="6" t="s">
-        <v>205</v>
-      </c>
-      <c r="N70" s="11" t="n">
+        <v>206</v>
+      </c>
+      <c r="N70" s="10" t="n">
         <f aca="false">D70=""</f>
         <v>1</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="6" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>170</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="D71" s="6"/>
       <c r="E71" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F71" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G71" s="6"/>
       <c r="H71" s="6"/>
@@ -3358,41 +3196,41 @@
     </row>
     <row r="72" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="B72" s="6" t="s">
         <v>170</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D72" s="6"/>
       <c r="E72" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F72" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G72" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H72" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I72" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J72" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K72" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L72" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M72" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N72" s="8" t="n">
         <f aca="false">D72=""</f>
@@ -3401,41 +3239,41 @@
     </row>
     <row r="73" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="B73" s="6" t="s">
         <v>170</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="D73" s="6"/>
       <c r="E73" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F73" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G73" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H73" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I73" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J73" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K73" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L73" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M73" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N73" s="8" t="n">
         <f aca="false">D73=""</f>
@@ -3444,41 +3282,41 @@
     </row>
     <row r="74" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B74" s="6" t="s">
         <v>170</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="D74" s="6"/>
       <c r="E74" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="F74" s="7" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G74" s="6" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="H74" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="I74" s="6" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="J74" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="K74" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L74" s="6" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="M74" s="6" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="N74" s="8" t="n">
         <f aca="false">D74=""</f>

</xml_diff>

<commit_message>
Brak danych ZUS nie jest już interpretowany jako bycie bezrobotnym.
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -205,15 +205,15 @@
     <t>NMB</t>
   </si>
   <si>
-    <t>Liczba miesięcy bycia bezrobotnym (bezrob lub brak danych ZUS).
-(za bezrobotnego uznajemy każdego z tytułem ubezpieczenia bezrob, bez względu na ew. inne tytuły ubezpieczenia w tym samym okresie oraz osoby w ogóle nie mające danych z ZUS dla danego okresu)</t>
+    <t>Liczba miesięcy bycia bezrobotnym (bezrob).
+(za bezrobotnego uznajemy każdego z tytułem ubezpieczenia bezrob, bez względu na ew. inne tytuły ubezpieczenia w tym samym okresie; braku danych ZUS nie uznajemy za bycie bezrobotnym)</t>
   </si>
   <si>
     <t>NMB_V2</t>
   </si>
   <si>
-    <t>Liczba miesięcy bycia bezrobotnym
-(za bezrobotnego uznajemy tylko osoby, które w danym okresie mają tytuł ubezpieczenia bezrob i jednocześnie nie mają żadnego tytułu ubezpieczenia etat/netat/samoze/rentemer/student albo w ogóle nie mają danych z ZUS dla danego okresu)</t>
+    <t>Liczba miesięcy bycia bezrobotnym (bezrob)
+(za bezrobotnego uznajemy tylko osoby, które w danym okresie mają tytuł ubezpieczenia bezrob i jednocześnie nie mają żadnego tytułu ubezpieczenia etat/netat/samoze/rentemer/student; braku danych ZUS nie uznajemy za bycie bezrobotnym)</t>
   </si>
   <si>
     <t>NME</t>
@@ -961,21 +961,20 @@
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D51" activeCellId="0" sqref="D51"/>
+      <selection pane="bottomLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="48.5969387755102"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="24.8367346938776"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="23.3520408163265"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.9234693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="24.5663265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1401,7 +1400,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>57</v>
       </c>
@@ -1717,7 +1716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="115.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="6" t="s">
         <v>78</v>
       </c>

</xml_diff>

<commit_message>
W związku ze zmianą sposobu wyliczania nmb, sposób wyliczania mnprd zmieniony na mnprd = (len - nmp) / len
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -504,7 +504,7 @@
   </si>
   <si>
     <t>Odsetek miesięcy pozostawania bez pracy w okienku.
-NMB / LEN
+(LEN – NMP) / LEN
 (NA dla 0/0)</t>
   </si>
   <si>
@@ -961,20 +961,21 @@
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C44" activeCellId="0" sqref="C44"/>
+      <selection pane="bottomLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.9234693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="24.5663265306122"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.2448979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="24.3010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
- Porównanie ze zbiorem MS uzupełnione o wiele nowych zmiennych. - Rozmaite korekty wynikające z porównania. - Dorzucenie do repo publicznych danych (PNA, powiaty, bezrobocie, itp.)
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -19,6 +19,30 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author/>
+  </authors>
+  <commentList>
+    <comment ref="C70" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Potrzeba dokładniejszego opisu, co uznajemy za kontynuację (jaką zależność czasową)</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="215">
   <si>
@@ -610,7 +634,7 @@
     <t>CZASPRUD_V2</t>
   </si>
   <si>
-    <t>Okres składkowy podjęcia pierwszej pracy etatowej (etat) jako  minus miesiąc uzyskania dyplomu (czas do podejęcia pierwszej pracy etatowek)
+    <t>Okres składkowy podjęcia pierwszej pracy etatowej (etat) minus miesiąc uzyskania dyplomu (czas do podejęcia pierwszej pracy etatowek)
 Wartość 0 tylko gdy utrzymał pracę o tym samym charakterze u tego samego pracodawcy w kolejnym miesiącu.</t>
   </si>
   <si>
@@ -772,7 +796,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -789,6 +813,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFEFEFEF"/>
         <bgColor rgb="FFEEEEEE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -840,7 +870,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -875,6 +905,14 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -961,21 +999,21 @@
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C49" activeCellId="0" sqref="C49"/>
+      <selection pane="bottomLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="47.2448979591837"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="14.5816326530612"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="24.3010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="22.6785714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4438775510204"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="45.6275510204082"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="23.0816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8673469387755"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.02551020408163"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2766,7 +2804,7 @@
       <c r="B58" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C58" s="6" t="s">
+      <c r="C58" s="9" t="s">
         <v>170</v>
       </c>
       <c r="D58" s="6"/>
@@ -2795,7 +2833,7 @@
       <c r="B59" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="9" t="s">
         <v>174</v>
       </c>
       <c r="D59" s="6"/>
@@ -2824,7 +2862,7 @@
       <c r="B60" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="9" t="s">
         <v>176</v>
       </c>
       <c r="D60" s="6"/>
@@ -2853,7 +2891,7 @@
       <c r="B61" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="9" t="s">
         <v>178</v>
       </c>
       <c r="D61" s="6"/>
@@ -2882,7 +2920,7 @@
       <c r="B62" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="9" t="s">
         <v>180</v>
       </c>
       <c r="D62" s="6"/>
@@ -2911,7 +2949,7 @@
       <c r="B63" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="9" t="s">
         <v>182</v>
       </c>
       <c r="D63" s="6"/>
@@ -3119,14 +3157,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="6" t="s">
         <v>195</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="10" t="s">
         <v>196</v>
       </c>
       <c r="D70" s="6"/>
@@ -3157,7 +3195,7 @@
       <c r="M70" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="N70" s="9" t="n">
+      <c r="N70" s="11" t="n">
         <f aca="false">D70=""</f>
         <v>1</v>
       </c>
@@ -3345,5 +3383,6 @@
   <colBreaks count="1" manualBreakCount="1">
     <brk id="13" man="true" max="65535" min="0"/>
   </colBreaks>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
len doprowadzone do zgodności (walki z "koniec" oraz z poprawnym dołączaniem "len" do innych zmiennych okienka czasu)
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -64,6 +64,9 @@
     <t>zbiór bazowy</t>
   </si>
   <si>
+    <t>wartość 0</t>
+  </si>
+  <si>
     <t>wartość 1</t>
   </si>
   <si>
@@ -80,9 +83,6 @@
   </si>
   <si>
     <t>wartość 6</t>
-  </si>
-  <si>
-    <t>wartość 7</t>
   </si>
   <si>
     <t>niezależna</t>
@@ -870,7 +870,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -905,10 +905,6 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -999,24 +995,25 @@
   <dimension ref="A1:N65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A57" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A63" activeCellId="0" sqref="A63"/>
+      <selection pane="bottomLeft" activeCell="L72" activeCellId="0" sqref="L72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="45.6275510204082"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="23.0816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.8673469387755"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="9.02551020408163"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.9540816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="22.8112244897959"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="13" min="8" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2804,7 +2801,7 @@
       <c r="B58" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C58" s="9" t="s">
+      <c r="C58" s="6" t="s">
         <v>170</v>
       </c>
       <c r="D58" s="6"/>
@@ -2833,7 +2830,7 @@
       <c r="B59" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C59" s="9" t="s">
+      <c r="C59" s="6" t="s">
         <v>174</v>
       </c>
       <c r="D59" s="6"/>
@@ -2862,7 +2859,7 @@
       <c r="B60" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C60" s="9" t="s">
+      <c r="C60" s="6" t="s">
         <v>176</v>
       </c>
       <c r="D60" s="6"/>
@@ -2891,7 +2888,7 @@
       <c r="B61" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C61" s="9" t="s">
+      <c r="C61" s="6" t="s">
         <v>178</v>
       </c>
       <c r="D61" s="6"/>
@@ -2920,7 +2917,7 @@
       <c r="B62" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C62" s="9" t="s">
+      <c r="C62" s="6" t="s">
         <v>180</v>
       </c>
       <c r="D62" s="6"/>
@@ -2949,7 +2946,7 @@
       <c r="B63" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C63" s="9" t="s">
+      <c r="C63" s="6" t="s">
         <v>182</v>
       </c>
       <c r="D63" s="6"/>
@@ -3164,7 +3161,7 @@
       <c r="B70" s="6" t="s">
         <v>169</v>
       </c>
-      <c r="C70" s="10" t="s">
+      <c r="C70" s="9" t="s">
         <v>196</v>
       </c>
       <c r="D70" s="6"/>
@@ -3195,7 +3192,7 @@
       <c r="M70" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="N70" s="11" t="n">
+      <c r="N70" s="10" t="n">
         <f aca="false">D70=""</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
- dodanie funkcji okres2miesiac() - dodanie funkcji oblicz_stale_czasowe() - zmiana nazw zmiennych KLASAZAM -> KLASZAM
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -13,7 +13,7 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="Unspecified"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1"/>
     </ext>
   </extLst>
 </workbook>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="215">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="226">
   <si>
     <t>zmienna</t>
   </si>
@@ -740,6 +740,39 @@
   </si>
   <si>
     <t>Charakter pierwszych napotkanych (wszystko jedno jakich) studiów jednolitych magisterskich odbywanych równolegle z uzyskaniem dyplomu</t>
+  </si>
+  <si>
+    <t>MCSTART</t>
+  </si>
+  <si>
+    <t>Miesiąc rozpoczęcia studiów</t>
+  </si>
+  <si>
+    <t>DATA_ZAK</t>
+  </si>
+  <si>
+    <t>oblicz_stale_czasowe</t>
+  </si>
+  <si>
+    <t>ROKSTART</t>
+  </si>
+  <si>
+    <t>Rok rozpoczęcia studiów</t>
+  </si>
+  <si>
+    <t>MCDYP</t>
+  </si>
+  <si>
+    <t>Miesiąc uzyskania dyplomu</t>
+  </si>
+  <si>
+    <t>DATA_ROZP</t>
+  </si>
+  <si>
+    <t>ROKDYP</t>
+  </si>
+  <si>
+    <t>Rok uzyskania dyplomu</t>
   </si>
 </sst>
 </file>
@@ -750,7 +783,7 @@
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="&quot;PRAWDA&quot;;&quot;PRAWDA&quot;;&quot;FAŁSZ&quot;"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -772,13 +805,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -870,28 +896,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -903,7 +929,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -911,8 +937,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -992,25 +1022,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N65536"/>
+  <dimension ref="A1:N78"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A73" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L72" activeCellId="0" sqref="L72"/>
+      <selection pane="bottomLeft" activeCell="C77" activeCellId="0" sqref="C77:C78"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.9540816326531"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.5"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="22.8112244897959"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="8" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.9030612244898"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="44.4132653061225"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="2" width="22.5459183673469"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.3265306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="8" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1057,7 +1088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="70.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
@@ -1086,7 +1117,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="6" t="s">
         <v>19</v>
       </c>
@@ -1112,7 +1143,7 @@
       <c r="M3" s="6"/>
       <c r="N3" s="8"/>
     </row>
-    <row r="4" customFormat="false" ht="35.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
@@ -1140,7 +1171,7 @@
       <c r="M4" s="6"/>
       <c r="N4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="6" t="s">
         <v>26</v>
       </c>
@@ -1168,7 +1199,7 @@
       <c r="M5" s="6"/>
       <c r="N5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>29</v>
       </c>
@@ -1196,7 +1227,7 @@
       <c r="M6" s="6"/>
       <c r="N6" s="8"/>
     </row>
-    <row r="7" customFormat="false" ht="47.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
         <v>32</v>
       </c>
@@ -1225,7 +1256,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="47.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="6" t="s">
         <v>35</v>
       </c>
@@ -1254,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>37</v>
       </c>
@@ -1285,7 +1316,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>40</v>
       </c>
@@ -1320,7 +1351,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>45</v>
       </c>
@@ -1349,7 +1380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>49</v>
       </c>
@@ -1378,7 +1409,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
@@ -1407,7 +1438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="47.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>54</v>
       </c>
@@ -1494,7 +1525,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
         <v>61</v>
       </c>
@@ -1523,7 +1554,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>63</v>
       </c>
@@ -1552,7 +1583,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>65</v>
       </c>
@@ -1581,7 +1612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>67</v>
       </c>
@@ -1610,7 +1641,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="6" t="s">
         <v>69</v>
       </c>
@@ -1639,7 +1670,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
         <v>71</v>
       </c>
@@ -1668,7 +1699,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="24.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
         <v>42</v>
       </c>
@@ -1783,7 +1814,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="104.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="6" t="s">
         <v>81</v>
       </c>
@@ -1814,7 +1845,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="115.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="6" t="s">
         <v>83</v>
       </c>
@@ -1876,7 +1907,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
         <v>88</v>
       </c>
@@ -2318,7 +2349,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
         <v>127</v>
       </c>
@@ -2355,7 +2386,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
         <v>135</v>
       </c>
@@ -2392,7 +2423,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
         <v>140</v>
       </c>
@@ -2429,7 +2460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="6" t="s">
         <v>142</v>
       </c>
@@ -2466,7 +2497,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="6" t="s">
         <v>145</v>
       </c>
@@ -2666,7 +2697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="6" t="s">
         <v>161</v>
       </c>
@@ -2697,7 +2728,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="47.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="6" t="s">
         <v>163</v>
       </c>
@@ -2728,7 +2759,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="6" t="s">
         <v>129</v>
       </c>
@@ -3226,7 +3257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A72" s="6" t="s">
         <v>208</v>
       </c>
@@ -3269,7 +3300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="6" t="s">
         <v>211</v>
       </c>
@@ -3312,7 +3343,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="6" t="s">
         <v>213</v>
       </c>
@@ -3355,20 +3386,118 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1048563" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048564" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048565" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048566" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048567" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="10" t="s">
+        <v>215</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>216</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="E75" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+      <c r="J75" s="10"/>
+      <c r="K75" s="10"/>
+      <c r="L75" s="10"/>
+      <c r="M75" s="10"/>
+      <c r="N75" s="10"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>220</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>217</v>
+      </c>
+      <c r="E76" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G76" s="10"/>
+      <c r="H76" s="10"/>
+      <c r="I76" s="10"/>
+      <c r="J76" s="10"/>
+      <c r="K76" s="10"/>
+      <c r="L76" s="10"/>
+      <c r="M76" s="10"/>
+      <c r="N76" s="10"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="10" t="s">
+        <v>221</v>
+      </c>
+      <c r="B77" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C77" s="10" t="s">
+        <v>222</v>
+      </c>
+      <c r="D77" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E77" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F77" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G77" s="10"/>
+      <c r="H77" s="10"/>
+      <c r="I77" s="10"/>
+      <c r="J77" s="10"/>
+      <c r="K77" s="10"/>
+      <c r="L77" s="10"/>
+      <c r="M77" s="10"/>
+      <c r="N77" s="10"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="B78" s="10" t="s">
+        <v>169</v>
+      </c>
+      <c r="C78" s="10" t="s">
+        <v>225</v>
+      </c>
+      <c r="D78" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="E78" s="11" t="s">
+        <v>218</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G78" s="10"/>
+      <c r="H78" s="10"/>
+      <c r="I78" s="10"/>
+      <c r="J78" s="10"/>
+      <c r="K78" s="10"/>
+      <c r="L78" s="10"/>
+      <c r="M78" s="10"/>
+      <c r="N78" s="10"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Dodanie zestawu zmiennych określających wysokopoziomowe statusy respondentów.
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -16,6 +16,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Arkusz1!$A$1:$P$86</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Arkusz1!$A$1:$P$86</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Arkusz1!$A$1:$P$86</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Arkusz1!$A$1:$P$86</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Arkusz1!$A$1:$P$86</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -51,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="735" uniqueCount="329">
   <si>
     <t xml:space="preserve">zmienna</t>
   </si>
@@ -253,11 +255,11 @@
     <t xml:space="preserve">EZARD</t>
   </si>
   <si>
-    <t xml:space="preserve">(SZE + SZN) / NMP
+    <t xml:space="preserve">(SZE + SZN) / NMZ
 (NA dla 0/0)</t>
   </si>
   <si>
-    <t xml:space="preserve">SZ, NMP</t>
+    <t xml:space="preserve">SZ, NMZ</t>
   </si>
   <si>
     <t xml:space="preserve">EZARDA</t>
@@ -968,6 +970,138 @@
   </si>
   <si>
     <t xml:space="preserve">GEZBAZYD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMES / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy pracy na etacie (etat) i studiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNS / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iiczba miesięcy pracy tylko nie na etacie (etat, netat) i studiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMDZS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMDZS / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMDZS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy wychowywania dziecka (dziecko) i studiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMINNES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMINNES / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMINNES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy posiadania składek w ZUS z tytułów innych niż etat, netat, dziecko i bycie bezrobotnym (etat, netat, dziecko, bezrob) i studiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMBSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMBSS / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMBSS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy nieposiadania składek w ZUS pomimo bycia studentem (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMENS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMENS / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMENS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy pracy na etacie (etat) i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMNNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNNS / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iiczba miesięcy pracy tylko nie na etacie (etat, netat) i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMDZNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMDZNS / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMDZNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy wychowywania dziecka (dziecko) i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMINNENS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMINNENS / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMINNENS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy posiadania składek w ZUS z tytułów innych niż etat, netat, dziecko i bycie bezrobotnym (etat, netat, dziecko, bezrob) i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMBNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMBNS / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMBNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy bycia bezrobotnym (bezrob) i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMBSNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMBSNS / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMBSNS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy nieposiadania składek w ZUS i niestudiowania (student2)</t>
   </si>
 </sst>
 </file>
@@ -1225,27 +1359,27 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P86"/>
+  <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="G65" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="G99" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K67" activeCellId="0" sqref="K67"/>
+      <selection pane="bottomLeft" activeCell="C111" activeCellId="0" sqref="C111:F121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="41.8469387755102"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="24.4336734693878"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.8418367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="12.9132653061225"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.765306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="23.7602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.3061224489796"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="7.4234693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1766,7 +1900,7 @@
       </c>
       <c r="P15" s="10"/>
     </row>
-    <row r="16" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="6" t="s">
         <v>62</v>
       </c>
@@ -4230,7 +4364,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
         <v>282</v>
       </c>
@@ -4266,6 +4400,710 @@
       <c r="P86" s="9" t="s">
         <v>284</v>
       </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="9" t="s">
+        <v>285</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>286</v>
+      </c>
+      <c r="D87" s="9"/>
+      <c r="E87" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="F87" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G87" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H87" s="9"/>
+      <c r="I87" s="9"/>
+      <c r="J87" s="9"/>
+      <c r="K87" s="9"/>
+      <c r="L87" s="9"/>
+      <c r="M87" s="9"/>
+      <c r="N87" s="9"/>
+      <c r="O87" s="8" t="n">
+        <f aca="false">E87=""</f>
+        <v>0</v>
+      </c>
+      <c r="P87" s="9"/>
+    </row>
+    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="9" t="s">
+        <v>287</v>
+      </c>
+      <c r="B88" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C88" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="D88" s="9"/>
+      <c r="E88" s="9"/>
+      <c r="F88" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G88" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H88" s="9"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="9"/>
+      <c r="N88" s="9"/>
+      <c r="O88" s="8" t="n">
+        <f aca="false">E88=""</f>
+        <v>1</v>
+      </c>
+      <c r="P88" s="9"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="B89" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C89" s="6" t="s">
+        <v>290</v>
+      </c>
+      <c r="D89" s="9"/>
+      <c r="E89" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="F89" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H89" s="9"/>
+      <c r="I89" s="9"/>
+      <c r="J89" s="9"/>
+      <c r="K89" s="9"/>
+      <c r="L89" s="9"/>
+      <c r="M89" s="9"/>
+      <c r="N89" s="9"/>
+      <c r="O89" s="8" t="n">
+        <f aca="false">E89=""</f>
+        <v>0</v>
+      </c>
+      <c r="P89" s="9"/>
+    </row>
+    <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="B90" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="D90" s="9"/>
+      <c r="E90" s="9"/>
+      <c r="F90" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G90" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H90" s="9"/>
+      <c r="I90" s="9"/>
+      <c r="J90" s="9"/>
+      <c r="K90" s="9"/>
+      <c r="L90" s="9"/>
+      <c r="M90" s="9"/>
+      <c r="N90" s="9"/>
+      <c r="O90" s="8" t="n">
+        <f aca="false">E90=""</f>
+        <v>1</v>
+      </c>
+      <c r="P90" s="9"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="9" t="s">
+        <v>293</v>
+      </c>
+      <c r="B91" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D91" s="9"/>
+      <c r="E91" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="F91" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H91" s="9"/>
+      <c r="I91" s="9"/>
+      <c r="J91" s="9"/>
+      <c r="K91" s="9"/>
+      <c r="L91" s="9"/>
+      <c r="M91" s="9"/>
+      <c r="N91" s="9"/>
+      <c r="O91" s="8" t="n">
+        <f aca="false">E91=""</f>
+        <v>0</v>
+      </c>
+      <c r="P91" s="9"/>
+    </row>
+    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="B92" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>296</v>
+      </c>
+      <c r="D92" s="9"/>
+      <c r="E92" s="9"/>
+      <c r="F92" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G92" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H92" s="9"/>
+      <c r="I92" s="9"/>
+      <c r="J92" s="9"/>
+      <c r="K92" s="9"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="9"/>
+      <c r="O92" s="8" t="n">
+        <f aca="false">E92=""</f>
+        <v>1</v>
+      </c>
+      <c r="P92" s="9"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="9" t="s">
+        <v>297</v>
+      </c>
+      <c r="B93" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C93" s="9" t="s">
+        <v>298</v>
+      </c>
+      <c r="D93" s="9"/>
+      <c r="E93" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="F93" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G93" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H93" s="9"/>
+      <c r="I93" s="9"/>
+      <c r="J93" s="9"/>
+      <c r="K93" s="9"/>
+      <c r="L93" s="9"/>
+      <c r="M93" s="9"/>
+      <c r="N93" s="9"/>
+      <c r="O93" s="8" t="n">
+        <f aca="false">E93=""</f>
+        <v>0</v>
+      </c>
+      <c r="P93" s="9"/>
+    </row>
+    <row r="94" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="9" t="s">
+        <v>299</v>
+      </c>
+      <c r="B94" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>300</v>
+      </c>
+      <c r="D94" s="9"/>
+      <c r="E94" s="9"/>
+      <c r="F94" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G94" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H94" s="9"/>
+      <c r="I94" s="9"/>
+      <c r="J94" s="9"/>
+      <c r="K94" s="9"/>
+      <c r="L94" s="9"/>
+      <c r="M94" s="9"/>
+      <c r="N94" s="9"/>
+      <c r="O94" s="8" t="n">
+        <f aca="false">E94=""</f>
+        <v>1</v>
+      </c>
+      <c r="P94" s="9"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="9" t="s">
+        <v>301</v>
+      </c>
+      <c r="B95" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C95" s="9" t="s">
+        <v>302</v>
+      </c>
+      <c r="D95" s="9"/>
+      <c r="E95" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="F95" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G95" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95" s="9"/>
+      <c r="I95" s="9"/>
+      <c r="J95" s="9"/>
+      <c r="K95" s="9"/>
+      <c r="L95" s="9"/>
+      <c r="M95" s="9"/>
+      <c r="N95" s="9"/>
+      <c r="O95" s="8" t="n">
+        <f aca="false">E95=""</f>
+        <v>0</v>
+      </c>
+      <c r="P95" s="9"/>
+    </row>
+    <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>304</v>
+      </c>
+      <c r="D96" s="9"/>
+      <c r="E96" s="9"/>
+      <c r="F96" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G96" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H96" s="9"/>
+      <c r="I96" s="9"/>
+      <c r="J96" s="9"/>
+      <c r="K96" s="9"/>
+      <c r="L96" s="9"/>
+      <c r="M96" s="9"/>
+      <c r="N96" s="9"/>
+      <c r="O96" s="8" t="n">
+        <f aca="false">E96=""</f>
+        <v>1</v>
+      </c>
+      <c r="P96" s="9"/>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="9" t="s">
+        <v>305</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C97" s="9" t="s">
+        <v>306</v>
+      </c>
+      <c r="D97" s="9"/>
+      <c r="E97" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="F97" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H97" s="9"/>
+      <c r="I97" s="9"/>
+      <c r="J97" s="9"/>
+      <c r="K97" s="9"/>
+      <c r="L97" s="9"/>
+      <c r="M97" s="9"/>
+      <c r="N97" s="9"/>
+      <c r="O97" s="8" t="n">
+        <f aca="false">E97=""</f>
+        <v>0</v>
+      </c>
+      <c r="P97" s="9"/>
+    </row>
+    <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="9" t="s">
+        <v>307</v>
+      </c>
+      <c r="B98" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C98" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D98" s="9"/>
+      <c r="E98" s="9"/>
+      <c r="F98" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G98" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H98" s="9"/>
+      <c r="I98" s="9"/>
+      <c r="J98" s="9"/>
+      <c r="K98" s="9"/>
+      <c r="L98" s="9"/>
+      <c r="M98" s="9"/>
+      <c r="N98" s="9"/>
+      <c r="O98" s="8" t="n">
+        <f aca="false">E98=""</f>
+        <v>1</v>
+      </c>
+      <c r="P98" s="9"/>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="B99" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C99" s="9" t="s">
+        <v>310</v>
+      </c>
+      <c r="D99" s="9"/>
+      <c r="E99" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H99" s="9"/>
+      <c r="I99" s="9"/>
+      <c r="J99" s="9"/>
+      <c r="K99" s="9"/>
+      <c r="L99" s="9"/>
+      <c r="M99" s="9"/>
+      <c r="N99" s="9"/>
+      <c r="O99" s="8" t="n">
+        <f aca="false">E99=""</f>
+        <v>0</v>
+      </c>
+      <c r="P99" s="9"/>
+    </row>
+    <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="9" t="s">
+        <v>311</v>
+      </c>
+      <c r="B100" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C100" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="D100" s="9"/>
+      <c r="E100" s="9"/>
+      <c r="F100" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G100" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H100" s="9"/>
+      <c r="I100" s="9"/>
+      <c r="J100" s="9"/>
+      <c r="K100" s="9"/>
+      <c r="L100" s="9"/>
+      <c r="M100" s="9"/>
+      <c r="N100" s="9"/>
+      <c r="O100" s="8" t="n">
+        <f aca="false">E100=""</f>
+        <v>1</v>
+      </c>
+      <c r="P100" s="9"/>
+    </row>
+    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="9" t="s">
+        <v>313</v>
+      </c>
+      <c r="B101" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C101" s="9" t="s">
+        <v>314</v>
+      </c>
+      <c r="D101" s="9"/>
+      <c r="E101" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="F101" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H101" s="9"/>
+      <c r="I101" s="9"/>
+      <c r="J101" s="9"/>
+      <c r="K101" s="9"/>
+      <c r="L101" s="9"/>
+      <c r="M101" s="9"/>
+      <c r="N101" s="9"/>
+      <c r="O101" s="8" t="n">
+        <f aca="false">E101=""</f>
+        <v>0</v>
+      </c>
+      <c r="P101" s="9"/>
+    </row>
+    <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A102" s="9" t="s">
+        <v>315</v>
+      </c>
+      <c r="B102" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C102" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="D102" s="9"/>
+      <c r="E102" s="9"/>
+      <c r="F102" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G102" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H102" s="9"/>
+      <c r="I102" s="9"/>
+      <c r="J102" s="9"/>
+      <c r="K102" s="9"/>
+      <c r="L102" s="9"/>
+      <c r="M102" s="9"/>
+      <c r="N102" s="9"/>
+      <c r="O102" s="8" t="n">
+        <f aca="false">E102=""</f>
+        <v>1</v>
+      </c>
+      <c r="P102" s="9"/>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="B103" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C103" s="9" t="s">
+        <v>318</v>
+      </c>
+      <c r="D103" s="9"/>
+      <c r="E103" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="F103" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H103" s="9"/>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="9"/>
+      <c r="M103" s="9"/>
+      <c r="N103" s="9"/>
+      <c r="O103" s="8" t="n">
+        <f aca="false">E103=""</f>
+        <v>0</v>
+      </c>
+      <c r="P103" s="9"/>
+    </row>
+    <row r="104" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="9" t="s">
+        <v>319</v>
+      </c>
+      <c r="B104" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="D104" s="9"/>
+      <c r="E104" s="9"/>
+      <c r="F104" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G104" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H104" s="9"/>
+      <c r="I104" s="9"/>
+      <c r="J104" s="9"/>
+      <c r="K104" s="9"/>
+      <c r="L104" s="9"/>
+      <c r="M104" s="9"/>
+      <c r="N104" s="9"/>
+      <c r="O104" s="8" t="n">
+        <f aca="false">E104=""</f>
+        <v>1</v>
+      </c>
+      <c r="P104" s="9"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="B105" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C105" s="9" t="s">
+        <v>322</v>
+      </c>
+      <c r="D105" s="9"/>
+      <c r="E105" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="F105" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G105" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H105" s="9"/>
+      <c r="I105" s="9"/>
+      <c r="J105" s="9"/>
+      <c r="K105" s="9"/>
+      <c r="L105" s="9"/>
+      <c r="M105" s="9"/>
+      <c r="N105" s="9"/>
+      <c r="O105" s="8" t="n">
+        <f aca="false">E105=""</f>
+        <v>0</v>
+      </c>
+      <c r="P105" s="9"/>
+    </row>
+    <row r="106" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="9" t="s">
+        <v>323</v>
+      </c>
+      <c r="B106" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="D106" s="9"/>
+      <c r="E106" s="9"/>
+      <c r="F106" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G106" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H106" s="9"/>
+      <c r="I106" s="9"/>
+      <c r="J106" s="9"/>
+      <c r="K106" s="9"/>
+      <c r="L106" s="9"/>
+      <c r="M106" s="9"/>
+      <c r="N106" s="9"/>
+      <c r="O106" s="8" t="n">
+        <f aca="false">E106=""</f>
+        <v>1</v>
+      </c>
+      <c r="P106" s="9"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="9" t="s">
+        <v>325</v>
+      </c>
+      <c r="B107" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C107" s="9" t="s">
+        <v>326</v>
+      </c>
+      <c r="D107" s="9"/>
+      <c r="E107" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="F107" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G107" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H107" s="9"/>
+      <c r="I107" s="9"/>
+      <c r="J107" s="9"/>
+      <c r="K107" s="9"/>
+      <c r="L107" s="9"/>
+      <c r="M107" s="9"/>
+      <c r="N107" s="9"/>
+      <c r="O107" s="8" t="n">
+        <f aca="false">E107=""</f>
+        <v>0</v>
+      </c>
+      <c r="P107" s="9"/>
+    </row>
+    <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D108" s="9"/>
+      <c r="E108" s="9"/>
+      <c r="F108" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G108" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H108" s="9"/>
+      <c r="I108" s="9"/>
+      <c r="J108" s="9"/>
+      <c r="K108" s="9"/>
+      <c r="L108" s="9"/>
+      <c r="M108" s="9"/>
+      <c r="N108" s="9"/>
+      <c r="O108" s="8" t="n">
+        <f aca="false">E108=""</f>
+        <v>1</v>
+      </c>
+      <c r="P108" s="9"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:P86"/>

</xml_diff>

<commit_message>
Dodane definicje zmiennych z wydania 0.5.0
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -18,6 +18,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">Arkusz1!$A$1:$P$86</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">Arkusz1!$A$1:$P$86</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">Arkusz1!$A$1:$P$86</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">Arkusz1!$A$1:$P$86</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -615,6 +616,42 @@
     <t xml:space="preserve">Liczba miesięcy bycia zatrudnionym bez etatu (netat)</t>
   </si>
   <si>
+    <t xml:space="preserve">NMNSTUDBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy nieposiadania składek w ZUS i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDBEZROB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy bycia bezrobotnym (bezrob) i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDDZIECKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy wychowywania dziecka (dziecko) i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDETAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy pracy na etacie (etat) i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDINNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy posiadania składek w ZUS z tytułów innych niż etat, netat, dziecko i bycie bezrobotnym (etat, netat, dziecko, bezrob) i niestudiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDNETAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iiczba miesięcy pracy tylko nie na etacie (etat, netat) i niestudiowania (student2)</t>
+  </si>
+  <si>
     <t xml:space="preserve">NMP</t>
   </si>
   <si>
@@ -625,6 +662,36 @@
   </si>
   <si>
     <t xml:space="preserve">Liczba miesięcy bycia samozatrudnionym (samoz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy nieposiadania składek w ZUS pomimo bycia studentem (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDDZIECKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy wychowywania dziecka (dziecko) i studiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDETAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy pracy na etacie (etat) i studiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDINNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy posiadania składek w ZUS z tytułów innych niż etat, netat, dziecko i bycie bezrobotnym (etat, netat, dziecko, bezrob) i studiowania (student2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDNETAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">iiczba miesięcy pracy tylko nie na etacie (etat, netat) i studiowania (student2)</t>
   </si>
   <si>
     <t xml:space="preserve">NMZ</t>
@@ -704,6 +771,72 @@
     <t xml:space="preserve">Procent miesięcy, w których absolwent był zarejestrowany jako bezrobotny w okresie po miesiącu uzysk. dyplomu (wyłącznie) do końca obserwacji:
 100 * NMB_V2 / LEN
 (patrz BEZD_V2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMNSTUDBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDBD / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMNSTUDBEZROB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDBEZROB / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMNSTUDDZIECKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDDZIECKO / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMNSTUDETAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDETAT / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMNSTUDINNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDINNE / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMNSTUDNETAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMNSTUDNETAT / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMSTUDBD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDBD / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMSTUDDZIECKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDDZIECKO / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMSTUDETAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDETAT / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMSTUDINNE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDINNE / LEN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PMSTUDNETAT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NMSTUDNETAT / LEN</t>
   </si>
   <si>
     <t xml:space="preserve">Identyfikator powiatu zamieszkania na koniec okienka (wyjątek - w momencie uzyskania dyplomu dla okienka obejmującego cały okres od uzyskania dyplomu)
@@ -970,138 +1103,6 @@
   </si>
   <si>
     <t xml:space="preserve">GEZBAZYD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMES / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy pracy na etacie (etat) i studiowania (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMNS / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iiczba miesięcy pracy tylko nie na etacie (etat, netat) i studiowania (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMDZS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMDZS / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMDZS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy wychowywania dziecka (dziecko) i studiowania (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMINNES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMINNES / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMINNES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy posiadania składek w ZUS z tytułów innych niż etat, netat, dziecko i bycie bezrobotnym (etat, netat, dziecko, bezrob) i studiowania (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMBSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMBSS / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMBSS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy nieposiadania składek w ZUS pomimo bycia studentem (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMENS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMENS / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMENS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy pracy na etacie (etat) i niestudiowania (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMNNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMNNS / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMNNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">iiczba miesięcy pracy tylko nie na etacie (etat, netat) i niestudiowania (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMDZNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMDZNS / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMDZNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy wychowywania dziecka (dziecko) i niestudiowania (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMINNENS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMINNENS / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMINNENS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy posiadania składek w ZUS z tytułów innych niż etat, netat, dziecko i bycie bezrobotnym (etat, netat, dziecko, bezrob) i niestudiowania (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMBNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMBNS / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMBNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy bycia bezrobotnym (bezrob) i niestudiowania (student2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PMBSNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMBSNS / LEN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NMBSNS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy nieposiadania składek w ZUS i niestudiowania (student2)</t>
   </si>
 </sst>
 </file>
@@ -1362,24 +1363,25 @@
   <dimension ref="A1:P108"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="G99" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="G102" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C111" activeCellId="0" sqref="C111:F121"/>
+      <selection pane="bottomLeft" activeCell="A111" activeCellId="0" sqref="A111:P121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.765306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="4" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="23.7602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.3061224489796"/>
-    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="8.77551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="19.3112244897959"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="40.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="18.8877551020408"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="23.3520408163265"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="19.0357142857143"/>
+    <col collapsed="false" hidden="false" max="14" min="9" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="7.29081632653061"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1432,7 +1434,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="6" t="s">
         <v>16</v>
       </c>
@@ -1512,7 +1514,7 @@
       </c>
       <c r="P3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="6" t="s">
         <v>29</v>
       </c>
@@ -1655,7 +1657,7 @@
       </c>
       <c r="P8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="6" t="s">
         <v>41</v>
       </c>
@@ -1690,7 +1692,7 @@
       </c>
       <c r="P9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
@@ -1725,7 +1727,7 @@
       </c>
       <c r="P10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
@@ -1760,7 +1762,7 @@
       </c>
       <c r="P11" s="10"/>
     </row>
-    <row r="12" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
         <v>50</v>
       </c>
@@ -1795,7 +1797,7 @@
       </c>
       <c r="P12" s="10"/>
     </row>
-    <row r="13" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="6" t="s">
         <v>53</v>
       </c>
@@ -1830,7 +1832,7 @@
       </c>
       <c r="P13" s="10"/>
     </row>
-    <row r="14" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="6" t="s">
         <v>56</v>
       </c>
@@ -1865,7 +1867,7 @@
       </c>
       <c r="P14" s="10"/>
     </row>
-    <row r="15" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="6" t="s">
         <v>59</v>
       </c>
@@ -1935,7 +1937,7 @@
       </c>
       <c r="P16" s="10"/>
     </row>
-    <row r="17" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="6" t="s">
         <v>65</v>
       </c>
@@ -1972,7 +1974,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="6" t="s">
         <v>69</v>
       </c>
@@ -2009,7 +2011,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="6" t="s">
         <v>73</v>
       </c>
@@ -2044,7 +2046,7 @@
       </c>
       <c r="P19" s="10"/>
     </row>
-    <row r="20" customFormat="false" ht="125.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="124.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="6" t="s">
         <v>77</v>
       </c>
@@ -2118,7 +2120,7 @@
       </c>
       <c r="P21" s="10"/>
     </row>
-    <row r="22" customFormat="false" ht="158.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="158.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="6" t="s">
         <v>85</v>
       </c>
@@ -2157,7 +2159,7 @@
       </c>
       <c r="P22" s="10"/>
     </row>
-    <row r="23" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="6" t="s">
         <v>94</v>
       </c>
@@ -2198,7 +2200,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="6" t="s">
         <v>100</v>
       </c>
@@ -2237,7 +2239,7 @@
       </c>
       <c r="P24" s="10"/>
     </row>
-    <row r="25" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="6" t="s">
         <v>102</v>
       </c>
@@ -2373,7 +2375,7 @@
       <c r="O28" s="9"/>
       <c r="P28" s="10"/>
     </row>
-    <row r="29" customFormat="false" ht="113.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="6" t="s">
         <v>124</v>
       </c>
@@ -2414,7 +2416,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="6" t="s">
         <v>128</v>
       </c>
@@ -2453,7 +2455,7 @@
       </c>
       <c r="P30" s="10"/>
     </row>
-    <row r="31" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="6" t="s">
         <v>130</v>
       </c>
@@ -2488,7 +2490,7 @@
       </c>
       <c r="P31" s="10"/>
     </row>
-    <row r="32" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="6" t="s">
         <v>133</v>
       </c>
@@ -2624,7 +2626,7 @@
       </c>
       <c r="P35" s="10"/>
     </row>
-    <row r="36" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="6" t="s">
         <v>146</v>
       </c>
@@ -2657,7 +2659,7 @@
       </c>
       <c r="P36" s="10"/>
     </row>
-    <row r="37" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="6" t="s">
         <v>148</v>
       </c>
@@ -2698,7 +2700,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="6" t="s">
         <v>28</v>
       </c>
@@ -2731,7 +2733,7 @@
       </c>
       <c r="P38" s="10"/>
     </row>
-    <row r="39" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="6" t="s">
         <v>20</v>
       </c>
@@ -2764,7 +2766,7 @@
       </c>
       <c r="P39" s="10"/>
     </row>
-    <row r="40" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="6" t="s">
         <v>150</v>
       </c>
@@ -2797,7 +2799,7 @@
       </c>
       <c r="P40" s="10"/>
     </row>
-    <row r="41" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="6" t="s">
         <v>157</v>
       </c>
@@ -2830,7 +2832,7 @@
       </c>
       <c r="P41" s="10"/>
     </row>
-    <row r="42" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="6" t="s">
         <v>159</v>
       </c>
@@ -2863,7 +2865,7 @@
       </c>
       <c r="P42" s="10"/>
     </row>
-    <row r="43" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="6" t="s">
         <v>164</v>
       </c>
@@ -2896,7 +2898,7 @@
       </c>
       <c r="P43" s="10"/>
     </row>
-    <row r="44" customFormat="false" ht="46.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="6" t="s">
         <v>166</v>
       </c>
@@ -2931,7 +2933,7 @@
       </c>
       <c r="P44" s="10"/>
     </row>
-    <row r="45" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="6" t="s">
         <v>169</v>
       </c>
@@ -2964,7 +2966,7 @@
       </c>
       <c r="P45" s="10"/>
     </row>
-    <row r="46" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="6" t="s">
         <v>171</v>
       </c>
@@ -2997,8 +2999,8 @@
       </c>
       <c r="P46" s="10"/>
     </row>
-    <row r="47" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="6" t="s">
+    <row r="47" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
         <v>173</v>
       </c>
       <c r="B47" s="6" t="s">
@@ -3007,31 +3009,29 @@
       <c r="C47" s="6" t="s">
         <v>174</v>
       </c>
-      <c r="D47" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E47" s="6"/>
-      <c r="F47" s="7" t="s">
-        <v>143</v>
+      <c r="D47" s="9"/>
+      <c r="E47" s="9"/>
+      <c r="F47" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G47" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="6"/>
-      <c r="I47" s="6"/>
-      <c r="J47" s="6"/>
-      <c r="K47" s="6"/>
-      <c r="L47" s="6"/>
-      <c r="M47" s="6"/>
-      <c r="N47" s="6"/>
+      <c r="H47" s="9"/>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
       <c r="O47" s="8" t="n">
         <f aca="false">E47=""</f>
         <v>1</v>
       </c>
-      <c r="P47" s="10"/>
-    </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="6" t="s">
+      <c r="P47" s="9"/>
+    </row>
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="s">
         <v>175</v>
       </c>
       <c r="B48" s="6" t="s">
@@ -3040,31 +3040,29 @@
       <c r="C48" s="6" t="s">
         <v>176</v>
       </c>
-      <c r="D48" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E48" s="6"/>
-      <c r="F48" s="7" t="s">
-        <v>143</v>
+      <c r="D48" s="9"/>
+      <c r="E48" s="9"/>
+      <c r="F48" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G48" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="6"/>
-      <c r="I48" s="6"/>
-      <c r="J48" s="6"/>
-      <c r="K48" s="6"/>
-      <c r="L48" s="6"/>
-      <c r="M48" s="6"/>
-      <c r="N48" s="6"/>
+      <c r="H48" s="9"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
       <c r="O48" s="8" t="n">
         <f aca="false">E48=""</f>
         <v>1</v>
       </c>
-      <c r="P48" s="10"/>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="6" t="s">
+      <c r="P48" s="9"/>
+    </row>
+    <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="s">
         <v>177</v>
       </c>
       <c r="B49" s="6" t="s">
@@ -3073,31 +3071,29 @@
       <c r="C49" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="D49" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E49" s="6"/>
-      <c r="F49" s="7" t="s">
-        <v>143</v>
+      <c r="D49" s="9"/>
+      <c r="E49" s="9"/>
+      <c r="F49" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G49" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
-      <c r="M49" s="6"/>
-      <c r="N49" s="6"/>
+      <c r="H49" s="9"/>
+      <c r="I49" s="9"/>
+      <c r="J49" s="9"/>
+      <c r="K49" s="9"/>
+      <c r="L49" s="9"/>
+      <c r="M49" s="9"/>
+      <c r="N49" s="9"/>
       <c r="O49" s="8" t="n">
         <f aca="false">E49=""</f>
         <v>1</v>
       </c>
-      <c r="P49" s="10"/>
-    </row>
-    <row r="50" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="6" t="s">
+      <c r="P49" s="9"/>
+    </row>
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="s">
         <v>179</v>
       </c>
       <c r="B50" s="6" t="s">
@@ -3106,123 +3102,111 @@
       <c r="C50" s="6" t="s">
         <v>180</v>
       </c>
-      <c r="D50" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E50" s="6"/>
-      <c r="F50" s="7" t="s">
-        <v>181</v>
+      <c r="D50" s="9"/>
+      <c r="E50" s="9"/>
+      <c r="F50" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G50" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
+      <c r="H50" s="9"/>
+      <c r="I50" s="9"/>
+      <c r="J50" s="9"/>
+      <c r="K50" s="9"/>
+      <c r="L50" s="9"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="9"/>
       <c r="O50" s="8" t="n">
         <f aca="false">E50=""</f>
         <v>1</v>
       </c>
-      <c r="P50" s="10"/>
-    </row>
-    <row r="51" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="6" t="s">
+      <c r="P50" s="9"/>
+    </row>
+    <row r="51" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C51" s="6" t="s">
         <v>182</v>
       </c>
-      <c r="B51" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C51" s="6" t="s">
-        <v>183</v>
-      </c>
-      <c r="D51" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E51" s="6"/>
-      <c r="F51" s="7" t="s">
-        <v>181</v>
+      <c r="D51" s="9"/>
+      <c r="E51" s="9"/>
+      <c r="F51" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G51" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H51" s="6"/>
-      <c r="I51" s="6"/>
-      <c r="J51" s="6"/>
-      <c r="K51" s="6"/>
-      <c r="L51" s="6"/>
-      <c r="M51" s="6"/>
-      <c r="N51" s="6"/>
+      <c r="H51" s="9"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
       <c r="O51" s="8" t="n">
         <f aca="false">E51=""</f>
         <v>1</v>
       </c>
-      <c r="P51" s="10"/>
-    </row>
-    <row r="52" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="6" t="s">
+      <c r="P51" s="9"/>
+    </row>
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="B52" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C52" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="B52" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>185</v>
-      </c>
-      <c r="D52" s="12"/>
-      <c r="E52" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F52" s="7" t="s">
-        <v>120</v>
+      <c r="D52" s="9"/>
+      <c r="E52" s="9"/>
+      <c r="F52" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G52" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H52" s="6"/>
-      <c r="I52" s="6"/>
-      <c r="J52" s="6"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H52" s="9"/>
+      <c r="I52" s="9"/>
+      <c r="J52" s="9"/>
+      <c r="K52" s="9"/>
+      <c r="L52" s="9"/>
+      <c r="M52" s="9"/>
+      <c r="N52" s="9"/>
       <c r="O52" s="8" t="n">
         <f aca="false">E52=""</f>
-        <v>0</v>
-      </c>
-      <c r="P52" s="10"/>
-    </row>
-    <row r="53" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="P52" s="9"/>
+    </row>
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="B53" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="6" t="s">
         <v>186</v>
-      </c>
-      <c r="B53" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C53" s="6" t="s">
-        <v>187</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E53" s="6" t="s">
-        <v>173</v>
-      </c>
+      <c r="E53" s="6"/>
       <c r="F53" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="G53" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H53" s="6" t="s">
-        <v>151</v>
-      </c>
-      <c r="I53" s="6" t="s">
-        <v>152</v>
-      </c>
+        <v>17</v>
+      </c>
+      <c r="H53" s="6"/>
+      <c r="I53" s="6"/>
       <c r="J53" s="6"/>
       <c r="K53" s="6"/>
       <c r="L53" s="6"/>
@@ -3230,31 +3214,29 @@
       <c r="N53" s="6"/>
       <c r="O53" s="8" t="n">
         <f aca="false">E53=""</f>
-        <v>0</v>
-      </c>
-      <c r="P53" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P53" s="10"/>
+    </row>
+    <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="B54" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C54" s="6" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="54" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="B54" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="C54" s="6" t="s">
-        <v>190</v>
-      </c>
-      <c r="D54" s="6"/>
-      <c r="E54" s="6" t="s">
-        <v>75</v>
-      </c>
+      <c r="D54" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E54" s="6"/>
       <c r="F54" s="7" t="s">
-        <v>89</v>
+        <v>143</v>
       </c>
       <c r="G54" s="7" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="H54" s="6"/>
       <c r="I54" s="6"/>
@@ -3265,192 +3247,184 @@
       <c r="N54" s="6"/>
       <c r="O54" s="8" t="n">
         <f aca="false">E54=""</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P54" s="10"/>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="6" t="s">
-        <v>191</v>
+    <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>189</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>192</v>
+        <v>17</v>
       </c>
       <c r="C55" s="6" t="s">
-        <v>193</v>
-      </c>
-      <c r="D55" s="6"/>
-      <c r="E55" s="6"/>
-      <c r="F55" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="G55" s="7"/>
-      <c r="H55" s="6"/>
-      <c r="I55" s="6"/>
-      <c r="J55" s="6"/>
-      <c r="K55" s="6"/>
-      <c r="L55" s="6"/>
-      <c r="M55" s="6"/>
-      <c r="N55" s="6"/>
+        <v>190</v>
+      </c>
+      <c r="D55" s="9"/>
+      <c r="E55" s="9"/>
+      <c r="F55" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H55" s="9"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
       <c r="O55" s="8" t="n">
         <f aca="false">E55=""</f>
         <v>1</v>
       </c>
       <c r="P55" s="9"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="6" t="s">
-        <v>195</v>
+    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="s">
+        <v>191</v>
       </c>
       <c r="B56" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C56" s="6" t="s">
         <v>192</v>
       </c>
-      <c r="C56" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="D56" s="6"/>
-      <c r="E56" s="6"/>
-      <c r="F56" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="G56" s="7"/>
-      <c r="H56" s="6"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="6"/>
-      <c r="K56" s="6"/>
-      <c r="L56" s="6"/>
-      <c r="M56" s="6"/>
-      <c r="N56" s="6"/>
+      <c r="D56" s="9"/>
+      <c r="E56" s="9"/>
+      <c r="F56" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G56" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H56" s="9"/>
+      <c r="I56" s="9"/>
+      <c r="J56" s="9"/>
+      <c r="K56" s="9"/>
+      <c r="L56" s="9"/>
+      <c r="M56" s="9"/>
+      <c r="N56" s="9"/>
       <c r="O56" s="8" t="n">
         <f aca="false">E56=""</f>
         <v>1</v>
       </c>
       <c r="P56" s="9"/>
     </row>
-    <row r="57" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="6" t="s">
-        <v>197</v>
+    <row r="57" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="s">
+        <v>193</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>198</v>
-      </c>
-      <c r="D57" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E57" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F57" s="7" t="s">
-        <v>21</v>
+        <v>194</v>
+      </c>
+      <c r="D57" s="9"/>
+      <c r="E57" s="9"/>
+      <c r="F57" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G57" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H57" s="6"/>
-      <c r="I57" s="6"/>
-      <c r="J57" s="6"/>
-      <c r="K57" s="6"/>
-      <c r="L57" s="6"/>
-      <c r="M57" s="6"/>
-      <c r="N57" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H57" s="9"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
       <c r="O57" s="8" t="n">
         <f aca="false">E57=""</f>
-        <v>0</v>
-      </c>
-      <c r="P57" s="10"/>
-    </row>
-    <row r="58" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="6" t="s">
-        <v>199</v>
+        <v>1</v>
+      </c>
+      <c r="P57" s="9"/>
+    </row>
+    <row r="58" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="s">
+        <v>195</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C58" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="D58" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E58" s="6" t="s">
-        <v>132</v>
-      </c>
-      <c r="F58" s="7" t="s">
-        <v>21</v>
+        <v>196</v>
+      </c>
+      <c r="D58" s="9"/>
+      <c r="E58" s="9"/>
+      <c r="F58" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G58" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H58" s="6"/>
-      <c r="I58" s="6"/>
-      <c r="J58" s="6"/>
-      <c r="K58" s="6"/>
-      <c r="L58" s="6"/>
-      <c r="M58" s="6"/>
-      <c r="N58" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H58" s="9"/>
+      <c r="I58" s="9"/>
+      <c r="J58" s="9"/>
+      <c r="K58" s="9"/>
+      <c r="L58" s="9"/>
+      <c r="M58" s="9"/>
+      <c r="N58" s="9"/>
       <c r="O58" s="8" t="n">
         <f aca="false">E58=""</f>
-        <v>0</v>
-      </c>
-      <c r="P58" s="10"/>
-    </row>
-    <row r="59" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="6" t="s">
-        <v>88</v>
+        <v>1</v>
+      </c>
+      <c r="P58" s="9"/>
+    </row>
+    <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="s">
+        <v>197</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>86</v>
+        <v>17</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>201</v>
-      </c>
-      <c r="D59" s="6"/>
-      <c r="E59" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="F59" s="7" t="s">
-        <v>89</v>
+        <v>198</v>
+      </c>
+      <c r="D59" s="9"/>
+      <c r="E59" s="9"/>
+      <c r="F59" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G59" s="7" t="s">
-        <v>90</v>
-      </c>
-      <c r="H59" s="6"/>
-      <c r="I59" s="6"/>
-      <c r="J59" s="6"/>
-      <c r="K59" s="6"/>
-      <c r="L59" s="6"/>
-      <c r="M59" s="6"/>
-      <c r="N59" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H59" s="9"/>
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
       <c r="O59" s="8" t="n">
         <f aca="false">E59=""</f>
-        <v>0</v>
-      </c>
-      <c r="P59" s="10"/>
-    </row>
-    <row r="60" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="P59" s="9"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="6" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D60" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E60" s="6" t="s">
-        <v>204</v>
-      </c>
+      <c r="E60" s="6"/>
       <c r="F60" s="7" t="s">
-        <v>21</v>
+        <v>143</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H60" s="6"/>
       <c r="I60" s="6"/>
@@ -3461,33 +3435,29 @@
       <c r="N60" s="6"/>
       <c r="O60" s="8" t="n">
         <f aca="false">E60=""</f>
-        <v>0</v>
-      </c>
-      <c r="P60" s="9" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+      <c r="P60" s="10"/>
+    </row>
+    <row r="61" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="6" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="D61" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E61" s="6" t="s">
-        <v>208</v>
-      </c>
+      <c r="E61" s="6"/>
       <c r="F61" s="7" t="s">
-        <v>21</v>
+        <v>203</v>
       </c>
       <c r="G61" s="7" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="H61" s="6"/>
       <c r="I61" s="6"/>
@@ -3498,87 +3468,91 @@
       <c r="N61" s="6"/>
       <c r="O61" s="8" t="n">
         <f aca="false">E61=""</f>
-        <v>0</v>
-      </c>
-      <c r="P61" s="9" t="s">
-        <v>209</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="B62" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="P61" s="10"/>
+    </row>
+    <row r="62" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="B62" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="D62" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E62" s="6"/>
+      <c r="F62" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="G62" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="H62" s="6"/>
+      <c r="I62" s="6"/>
+      <c r="J62" s="6"/>
+      <c r="K62" s="6"/>
+      <c r="L62" s="6"/>
+      <c r="M62" s="6"/>
+      <c r="N62" s="6"/>
+      <c r="O62" s="8" t="n">
+        <f aca="false">E62=""</f>
+        <v>1</v>
+      </c>
+      <c r="P62" s="10"/>
+    </row>
+    <row r="63" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C62" s="9" t="s">
-        <v>211</v>
-      </c>
-      <c r="D62" s="9"/>
-      <c r="E62" s="9" t="s">
-        <v>119</v>
-      </c>
-      <c r="F62" s="11" t="s">
+      <c r="C63" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="D63" s="12"/>
+      <c r="E63" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="F63" s="7" t="s">
         <v>120</v>
       </c>
-      <c r="G62" s="11" t="s">
+      <c r="G63" s="7" t="s">
         <v>105</v>
       </c>
-      <c r="H62" s="9"/>
-      <c r="I62" s="9"/>
-      <c r="J62" s="9"/>
-      <c r="K62" s="9"/>
-      <c r="L62" s="9"/>
-      <c r="M62" s="9"/>
-      <c r="N62" s="9"/>
-      <c r="O62" s="9"/>
-      <c r="P62" s="10"/>
-    </row>
-    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="9" t="s">
-        <v>212</v>
-      </c>
-      <c r="B63" s="9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C63" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="D63" s="9"/>
-      <c r="E63" s="9" t="s">
-        <v>123</v>
-      </c>
-      <c r="F63" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="G63" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="H63" s="9"/>
-      <c r="I63" s="9"/>
-      <c r="J63" s="9"/>
-      <c r="K63" s="9"/>
-      <c r="L63" s="9"/>
-      <c r="M63" s="9"/>
-      <c r="N63" s="9"/>
-      <c r="O63" s="9"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+      <c r="J63" s="6"/>
+      <c r="K63" s="6"/>
+      <c r="L63" s="6"/>
+      <c r="M63" s="6"/>
+      <c r="N63" s="6"/>
+      <c r="O63" s="8" t="n">
+        <f aca="false">E63=""</f>
+        <v>0</v>
+      </c>
       <c r="P63" s="10"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="6" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="D64" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>175</v>
+        <v>185</v>
       </c>
       <c r="F64" s="7" t="s">
         <v>21</v>
@@ -3587,10 +3561,10 @@
         <v>22</v>
       </c>
       <c r="H64" s="6" t="s">
-        <v>23</v>
+        <v>151</v>
       </c>
       <c r="I64" s="6" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="J64" s="6"/>
       <c r="K64" s="6"/>
@@ -3602,26 +3576,28 @@
         <v>0</v>
       </c>
       <c r="P64" s="9" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="6" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="D65" s="6"/>
-      <c r="E65" s="6"/>
+      <c r="E65" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="F65" s="7" t="s">
-        <v>104</v>
+        <v>89</v>
       </c>
       <c r="G65" s="7" t="s">
-        <v>105</v>
+        <v>90</v>
       </c>
       <c r="H65" s="6"/>
       <c r="I65" s="6"/>
@@ -3632,164 +3608,124 @@
       <c r="N65" s="6"/>
       <c r="O65" s="8" t="n">
         <f aca="false">E65=""</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P65" s="10"/>
     </row>
-    <row r="66" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="6" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>33</v>
+        <v>214</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="D66" s="6"/>
       <c r="E66" s="6"/>
       <c r="F66" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G66" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H66" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="I66" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="J66" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="K66" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="L66" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M66" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="N66" s="6" t="s">
-        <v>112</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="G66" s="7"/>
+      <c r="H66" s="6"/>
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
+      <c r="M66" s="6"/>
+      <c r="N66" s="6"/>
       <c r="O66" s="8" t="n">
         <f aca="false">E66=""</f>
         <v>1</v>
       </c>
-      <c r="P66" s="10"/>
-    </row>
-    <row r="67" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P66" s="9"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="6" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>33</v>
+        <v>214</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D67" s="6"/>
       <c r="E67" s="6"/>
       <c r="F67" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="G67" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H67" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="I67" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="J67" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="K67" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="L67" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M67" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="N67" s="6" t="s">
-        <v>112</v>
-      </c>
+        <v>216</v>
+      </c>
+      <c r="G67" s="7"/>
+      <c r="H67" s="6"/>
+      <c r="I67" s="6"/>
+      <c r="J67" s="6"/>
+      <c r="K67" s="6"/>
+      <c r="L67" s="6"/>
+      <c r="M67" s="6"/>
+      <c r="N67" s="6"/>
       <c r="O67" s="8" t="n">
         <f aca="false">E67=""</f>
         <v>1</v>
       </c>
-      <c r="P67" s="10"/>
-    </row>
-    <row r="68" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P67" s="9"/>
+    </row>
+    <row r="68" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="6" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>225</v>
-      </c>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
+        <v>220</v>
+      </c>
+      <c r="D68" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E68" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="F68" s="7" t="s">
-        <v>104</v>
+        <v>21</v>
       </c>
       <c r="G68" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="H68" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="I68" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="J68" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="K68" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="L68" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="M68" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="N68" s="6" t="s">
-        <v>112</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="H68" s="6"/>
+      <c r="I68" s="6"/>
+      <c r="J68" s="6"/>
+      <c r="K68" s="6"/>
+      <c r="L68" s="6"/>
+      <c r="M68" s="6"/>
+      <c r="N68" s="6"/>
       <c r="O68" s="8" t="n">
         <f aca="false">E68=""</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P68" s="10"/>
     </row>
-    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="B69" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="E69" s="6"/>
+      <c r="E69" s="6" t="s">
+        <v>132</v>
+      </c>
       <c r="F69" s="7" t="s">
-        <v>143</v>
+        <v>21</v>
       </c>
       <c r="G69" s="7" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="H69" s="6"/>
       <c r="I69" s="6"/>
@@ -3800,410 +3736,392 @@
       <c r="N69" s="6"/>
       <c r="O69" s="8" t="n">
         <f aca="false">E69=""</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P69" s="10"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A70" s="6" t="s">
-        <v>228</v>
+      <c r="A70" s="0" t="s">
+        <v>223</v>
       </c>
       <c r="B70" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C70" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="D70" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E70" s="6"/>
-      <c r="F70" s="7" t="s">
-        <v>143</v>
+      <c r="C70" s="9" t="s">
+        <v>224</v>
+      </c>
+      <c r="D70" s="9"/>
+      <c r="E70" s="0" t="s">
+        <v>173</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G70" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H70" s="6"/>
-      <c r="I70" s="6"/>
-      <c r="J70" s="6"/>
-      <c r="K70" s="6"/>
-      <c r="L70" s="6"/>
-      <c r="M70" s="6"/>
-      <c r="N70" s="6"/>
+      <c r="H70" s="9"/>
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
       <c r="O70" s="8" t="n">
         <f aca="false">E70=""</f>
-        <v>1</v>
-      </c>
-      <c r="P70" s="10"/>
+        <v>0</v>
+      </c>
+      <c r="P70" s="9"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A71" s="6" t="s">
-        <v>230</v>
+      <c r="A71" s="0" t="s">
+        <v>225</v>
       </c>
       <c r="B71" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C71" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="D71" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E71" s="6"/>
-      <c r="F71" s="7" t="s">
-        <v>143</v>
+      <c r="C71" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="D71" s="9"/>
+      <c r="E71" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G71" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H71" s="6"/>
-      <c r="I71" s="6"/>
-      <c r="J71" s="6"/>
-      <c r="K71" s="6"/>
-      <c r="L71" s="6"/>
-      <c r="M71" s="6"/>
-      <c r="N71" s="6"/>
+      <c r="H71" s="9"/>
+      <c r="I71" s="9"/>
+      <c r="J71" s="9"/>
+      <c r="K71" s="9"/>
+      <c r="L71" s="9"/>
+      <c r="M71" s="9"/>
+      <c r="N71" s="9"/>
       <c r="O71" s="8" t="n">
         <f aca="false">E71=""</f>
-        <v>1</v>
-      </c>
-      <c r="P71" s="10"/>
-    </row>
-    <row r="72" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A72" s="6" t="s">
-        <v>232</v>
+        <v>0</v>
+      </c>
+      <c r="P71" s="9"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
+        <v>227</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C72" s="6" t="s">
-        <v>233</v>
-      </c>
-      <c r="D72" s="6"/>
-      <c r="E72" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="F72" s="7" t="s">
-        <v>139</v>
+        <v>17</v>
+      </c>
+      <c r="C72" s="9" t="s">
+        <v>228</v>
+      </c>
+      <c r="D72" s="9"/>
+      <c r="E72" s="0" t="s">
+        <v>177</v>
+      </c>
+      <c r="F72" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G72" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H72" s="6"/>
-      <c r="I72" s="6"/>
-      <c r="J72" s="6"/>
-      <c r="K72" s="6"/>
-      <c r="L72" s="6"/>
-      <c r="M72" s="6"/>
-      <c r="N72" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H72" s="9"/>
+      <c r="I72" s="9"/>
+      <c r="J72" s="9"/>
+      <c r="K72" s="9"/>
+      <c r="L72" s="9"/>
+      <c r="M72" s="9"/>
+      <c r="N72" s="9"/>
       <c r="O72" s="8" t="n">
         <f aca="false">E72=""</f>
         <v>0</v>
       </c>
-      <c r="P72" s="10" t="s">
-        <v>235</v>
-      </c>
-    </row>
-    <row r="73" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A73" s="6" t="s">
-        <v>138</v>
+      <c r="P72" s="9"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>229</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C73" s="6" t="s">
-        <v>236</v>
-      </c>
-      <c r="D73" s="6" t="s">
-        <v>237</v>
-      </c>
-      <c r="E73" s="6"/>
-      <c r="F73" s="7" t="s">
-        <v>139</v>
+        <v>17</v>
+      </c>
+      <c r="C73" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="D73" s="9"/>
+      <c r="E73" s="0" t="s">
+        <v>179</v>
+      </c>
+      <c r="F73" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G73" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H73" s="6"/>
-      <c r="I73" s="6"/>
-      <c r="J73" s="6"/>
-      <c r="K73" s="6"/>
-      <c r="L73" s="6"/>
-      <c r="M73" s="6"/>
-      <c r="N73" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H73" s="9"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
       <c r="O73" s="8" t="n">
         <f aca="false">E73=""</f>
-        <v>1</v>
-      </c>
-      <c r="P73" s="10" t="s">
-        <v>238</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A74" s="6" t="s">
-        <v>239</v>
+        <v>0</v>
+      </c>
+      <c r="P73" s="9"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>231</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C74" s="6" t="s">
-        <v>240</v>
-      </c>
-      <c r="D74" s="6"/>
-      <c r="E74" s="6" t="s">
-        <v>241</v>
-      </c>
-      <c r="F74" s="7" t="s">
-        <v>139</v>
+        <v>17</v>
+      </c>
+      <c r="C74" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="D74" s="9"/>
+      <c r="E74" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="F74" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G74" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H74" s="6"/>
-      <c r="I74" s="6"/>
-      <c r="J74" s="6"/>
-      <c r="K74" s="6"/>
-      <c r="L74" s="6"/>
-      <c r="M74" s="6"/>
-      <c r="N74" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H74" s="9"/>
+      <c r="I74" s="9"/>
+      <c r="J74" s="9"/>
+      <c r="K74" s="9"/>
+      <c r="L74" s="9"/>
+      <c r="M74" s="9"/>
+      <c r="N74" s="9"/>
       <c r="O74" s="8" t="n">
         <f aca="false">E74=""</f>
         <v>0</v>
       </c>
-      <c r="P74" s="10" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A75" s="6" t="s">
-        <v>241</v>
+      <c r="P74" s="9"/>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>233</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C75" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="D75" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="E75" s="6"/>
-      <c r="F75" s="7" t="s">
-        <v>139</v>
+        <v>17</v>
+      </c>
+      <c r="C75" s="9" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75" s="9"/>
+      <c r="E75" s="0" t="s">
+        <v>183</v>
+      </c>
+      <c r="F75" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G75" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H75" s="6"/>
-      <c r="I75" s="6"/>
-      <c r="J75" s="6"/>
-      <c r="K75" s="6"/>
-      <c r="L75" s="6"/>
-      <c r="M75" s="6"/>
-      <c r="N75" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H75" s="9"/>
+      <c r="I75" s="9"/>
+      <c r="J75" s="9"/>
+      <c r="K75" s="9"/>
+      <c r="L75" s="9"/>
+      <c r="M75" s="9"/>
+      <c r="N75" s="9"/>
       <c r="O75" s="8" t="n">
         <f aca="false">E75=""</f>
-        <v>1</v>
-      </c>
-      <c r="P75" s="10" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A76" s="6" t="s">
-        <v>246</v>
+        <v>0</v>
+      </c>
+      <c r="P75" s="9"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>235</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>247</v>
-      </c>
-      <c r="D76" s="6"/>
-      <c r="E76" s="6" t="s">
-        <v>248</v>
-      </c>
-      <c r="F76" s="7" t="s">
-        <v>139</v>
+        <v>17</v>
+      </c>
+      <c r="C76" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="D76" s="9"/>
+      <c r="E76" s="0" t="s">
+        <v>189</v>
+      </c>
+      <c r="F76" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G76" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H76" s="6"/>
-      <c r="I76" s="6"/>
-      <c r="J76" s="6"/>
-      <c r="K76" s="6"/>
-      <c r="L76" s="6"/>
-      <c r="M76" s="6"/>
-      <c r="N76" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H76" s="9"/>
+      <c r="I76" s="9"/>
+      <c r="J76" s="9"/>
+      <c r="K76" s="9"/>
+      <c r="L76" s="9"/>
+      <c r="M76" s="9"/>
+      <c r="N76" s="9"/>
       <c r="O76" s="8" t="n">
         <f aca="false">E76=""</f>
         <v>0</v>
       </c>
-      <c r="P76" s="10" t="s">
-        <v>249</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="80.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A77" s="6" t="s">
-        <v>248</v>
+      <c r="P76" s="9"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>237</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C77" s="6" t="s">
-        <v>250</v>
-      </c>
-      <c r="D77" s="6" t="s">
-        <v>251</v>
-      </c>
-      <c r="E77" s="6"/>
-      <c r="F77" s="7" t="s">
-        <v>139</v>
+        <v>238</v>
+      </c>
+      <c r="D77" s="9"/>
+      <c r="E77" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="F77" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G77" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H77" s="6"/>
-      <c r="I77" s="6"/>
-      <c r="J77" s="6"/>
-      <c r="K77" s="6"/>
-      <c r="L77" s="6"/>
-      <c r="M77" s="6"/>
-      <c r="N77" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H77" s="9"/>
+      <c r="I77" s="9"/>
+      <c r="J77" s="9"/>
+      <c r="K77" s="9"/>
+      <c r="L77" s="9"/>
+      <c r="M77" s="9"/>
+      <c r="N77" s="9"/>
       <c r="O77" s="8" t="n">
         <f aca="false">E77=""</f>
-        <v>1</v>
-      </c>
-      <c r="P77" s="10" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="78" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A78" s="6" t="s">
-        <v>253</v>
+        <v>0</v>
+      </c>
+      <c r="P77" s="9"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>239</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="D78" s="6"/>
-      <c r="E78" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="F78" s="7" t="s">
-        <v>139</v>
+        <v>240</v>
+      </c>
+      <c r="D78" s="9"/>
+      <c r="E78" s="0" t="s">
+        <v>193</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G78" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H78" s="6"/>
-      <c r="I78" s="6"/>
-      <c r="J78" s="6"/>
-      <c r="K78" s="6"/>
-      <c r="L78" s="6"/>
-      <c r="M78" s="6"/>
-      <c r="N78" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H78" s="9"/>
+      <c r="I78" s="9"/>
+      <c r="J78" s="9"/>
+      <c r="K78" s="9"/>
+      <c r="L78" s="9"/>
+      <c r="M78" s="9"/>
+      <c r="N78" s="9"/>
       <c r="O78" s="8" t="n">
         <f aca="false">E78=""</f>
         <v>0</v>
       </c>
-      <c r="P78" s="10" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="79" customFormat="false" ht="102.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A79" s="6" t="s">
-        <v>255</v>
+      <c r="P78" s="9"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>241</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>257</v>
-      </c>
-      <c r="D79" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="E79" s="6"/>
-      <c r="F79" s="7" t="s">
-        <v>139</v>
+        <v>17</v>
+      </c>
+      <c r="C79" s="9" t="s">
+        <v>242</v>
+      </c>
+      <c r="D79" s="9"/>
+      <c r="E79" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="F79" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G79" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H79" s="6"/>
-      <c r="I79" s="6"/>
-      <c r="J79" s="6"/>
-      <c r="K79" s="6"/>
-      <c r="L79" s="6"/>
-      <c r="M79" s="6"/>
-      <c r="N79" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H79" s="9"/>
+      <c r="I79" s="9"/>
+      <c r="J79" s="9"/>
+      <c r="K79" s="9"/>
+      <c r="L79" s="9"/>
+      <c r="M79" s="9"/>
+      <c r="N79" s="9"/>
       <c r="O79" s="8" t="n">
         <f aca="false">E79=""</f>
-        <v>1</v>
-      </c>
-      <c r="P79" s="10" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A80" s="6" t="s">
-        <v>260</v>
+        <v>0</v>
+      </c>
+      <c r="P79" s="9"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>243</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C80" s="6" t="s">
-        <v>261</v>
-      </c>
-      <c r="D80" s="6"/>
-      <c r="E80" s="6" t="s">
-        <v>262</v>
-      </c>
-      <c r="F80" s="7" t="s">
-        <v>139</v>
+        <v>244</v>
+      </c>
+      <c r="D80" s="9"/>
+      <c r="E80" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="F80" s="11" t="s">
+        <v>115</v>
       </c>
       <c r="G80" s="7" t="s">
-        <v>234</v>
-      </c>
-      <c r="H80" s="6"/>
-      <c r="I80" s="6"/>
-      <c r="J80" s="6"/>
-      <c r="K80" s="6"/>
-      <c r="L80" s="6"/>
-      <c r="M80" s="6"/>
-      <c r="N80" s="6"/>
+        <v>17</v>
+      </c>
+      <c r="H80" s="9"/>
+      <c r="I80" s="9"/>
+      <c r="J80" s="9"/>
+      <c r="K80" s="9"/>
+      <c r="L80" s="9"/>
+      <c r="M80" s="9"/>
+      <c r="N80" s="9"/>
       <c r="O80" s="8" t="n">
         <f aca="false">E80=""</f>
         <v>0</v>
       </c>
-      <c r="P80" s="10" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="81" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P80" s="9"/>
+    </row>
+    <row r="81" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="6" t="s">
-        <v>262</v>
+        <v>88</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>33</v>
+        <v>86</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>264</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>265</v>
-      </c>
-      <c r="E81" s="6"/>
+        <v>245</v>
+      </c>
+      <c r="D81" s="6"/>
+      <c r="E81" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="F81" s="7" t="s">
-        <v>139</v>
+        <v>89</v>
       </c>
       <c r="G81" s="7" t="s">
-        <v>234</v>
+        <v>90</v>
       </c>
       <c r="H81" s="6"/>
       <c r="I81" s="6"/>
@@ -4214,31 +4132,31 @@
       <c r="N81" s="6"/>
       <c r="O81" s="8" t="n">
         <f aca="false">E81=""</f>
-        <v>1</v>
-      </c>
-      <c r="P81" s="10" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="P81" s="10"/>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="6" t="s">
-        <v>267</v>
+        <v>246</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="D82" s="6"/>
+        <v>247</v>
+      </c>
+      <c r="D82" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="E82" s="6" t="s">
-        <v>269</v>
+        <v>248</v>
       </c>
       <c r="F82" s="7" t="s">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="G82" s="7" t="s">
-        <v>234</v>
+        <v>22</v>
       </c>
       <c r="H82" s="6"/>
       <c r="I82" s="6"/>
@@ -4251,29 +4169,31 @@
         <f aca="false">E82=""</f>
         <v>0</v>
       </c>
-      <c r="P82" s="10" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="P82" s="9" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="6" t="s">
-        <v>269</v>
+        <v>250</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>33</v>
+        <v>17</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>271</v>
+        <v>251</v>
       </c>
       <c r="D83" s="6" t="s">
-        <v>272</v>
-      </c>
-      <c r="E83" s="6"/>
+        <v>19</v>
+      </c>
+      <c r="E83" s="6" t="s">
+        <v>252</v>
+      </c>
       <c r="F83" s="7" t="s">
-        <v>139</v>
+        <v>21</v>
       </c>
       <c r="G83" s="7" t="s">
-        <v>234</v>
+        <v>22</v>
       </c>
       <c r="H83" s="6"/>
       <c r="I83" s="6"/>
@@ -4284,110 +4204,100 @@
       <c r="N83" s="6"/>
       <c r="O83" s="8" t="n">
         <f aca="false">E83=""</f>
-        <v>1</v>
-      </c>
-      <c r="P83" s="10" t="s">
-        <v>273</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A84" s="6" t="s">
-        <v>274</v>
-      </c>
-      <c r="B84" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>276</v>
-      </c>
-      <c r="F84" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G84" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H84" s="6"/>
-      <c r="I84" s="6"/>
-      <c r="J84" s="6"/>
-      <c r="K84" s="6"/>
-      <c r="L84" s="6"/>
-      <c r="M84" s="6"/>
-      <c r="N84" s="6"/>
-      <c r="O84" s="8" t="n">
-        <f aca="false">E84=""</f>
-        <v>0</v>
-      </c>
-      <c r="P84" s="9" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A85" s="6" t="s">
-        <v>278</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>279</v>
-      </c>
-      <c r="D85" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E85" s="6" t="s">
-        <v>280</v>
-      </c>
-      <c r="F85" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="G85" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H85" s="6"/>
-      <c r="I85" s="6"/>
-      <c r="J85" s="6"/>
-      <c r="K85" s="6"/>
-      <c r="L85" s="6"/>
-      <c r="M85" s="6"/>
-      <c r="N85" s="6"/>
-      <c r="O85" s="8" t="n">
-        <f aca="false">E85=""</f>
-        <v>0</v>
-      </c>
-      <c r="P85" s="9" t="s">
-        <v>281</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>0</v>
+      </c>
+      <c r="P83" s="9" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B84" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C84" s="9" t="s">
+        <v>255</v>
+      </c>
+      <c r="D84" s="9"/>
+      <c r="E84" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G84" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H84" s="9"/>
+      <c r="I84" s="9"/>
+      <c r="J84" s="9"/>
+      <c r="K84" s="9"/>
+      <c r="L84" s="9"/>
+      <c r="M84" s="9"/>
+      <c r="N84" s="9"/>
+      <c r="O84" s="9"/>
+      <c r="P84" s="10"/>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="9" t="s">
+        <v>256</v>
+      </c>
+      <c r="B85" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="C85" s="9" t="s">
+        <v>257</v>
+      </c>
+      <c r="D85" s="9"/>
+      <c r="E85" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="G85" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="H85" s="9"/>
+      <c r="I85" s="9"/>
+      <c r="J85" s="9"/>
+      <c r="K85" s="9"/>
+      <c r="L85" s="9"/>
+      <c r="M85" s="9"/>
+      <c r="N85" s="9"/>
+      <c r="O85" s="9"/>
+      <c r="P85" s="10"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A86" s="6" t="s">
-        <v>282</v>
+        <v>258</v>
       </c>
       <c r="B86" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C86" s="6" t="s">
-        <v>283</v>
+        <v>259</v>
       </c>
       <c r="D86" s="6" t="s">
         <v>19</v>
       </c>
       <c r="E86" s="6" t="s">
-        <v>75</v>
+        <v>187</v>
       </c>
       <c r="F86" s="7" t="s">
-        <v>76</v>
+        <v>21</v>
       </c>
       <c r="G86" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H86" s="6"/>
-      <c r="I86" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="H86" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="I86" s="6" t="s">
+        <v>24</v>
+      </c>
       <c r="J86" s="6"/>
       <c r="K86" s="6"/>
       <c r="L86" s="6"/>
@@ -4398,712 +4308,804 @@
         <v>0</v>
       </c>
       <c r="P86" s="9" t="s">
-        <v>284</v>
-      </c>
-    </row>
-    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A87" s="9" t="s">
-        <v>285</v>
+        <v>260</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="6" t="s">
+        <v>261</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C87" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="D87" s="9"/>
-      <c r="E87" s="9" t="s">
-        <v>287</v>
-      </c>
-      <c r="F87" s="11" t="s">
-        <v>115</v>
+        <v>262</v>
+      </c>
+      <c r="D87" s="6"/>
+      <c r="E87" s="6"/>
+      <c r="F87" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H87" s="9"/>
-      <c r="I87" s="9"/>
-      <c r="J87" s="9"/>
-      <c r="K87" s="9"/>
-      <c r="L87" s="9"/>
-      <c r="M87" s="9"/>
-      <c r="N87" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="H87" s="6"/>
+      <c r="I87" s="6"/>
+      <c r="J87" s="6"/>
+      <c r="K87" s="6"/>
+      <c r="L87" s="6"/>
+      <c r="M87" s="6"/>
+      <c r="N87" s="6"/>
       <c r="O87" s="8" t="n">
         <f aca="false">E87=""</f>
-        <v>0</v>
-      </c>
-      <c r="P87" s="9"/>
-    </row>
-    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A88" s="9" t="s">
-        <v>287</v>
+        <v>1</v>
+      </c>
+      <c r="P87" s="10"/>
+    </row>
+    <row r="88" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C88" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="D88" s="9"/>
-      <c r="E88" s="9"/>
-      <c r="F88" s="11" t="s">
-        <v>115</v>
+        <v>264</v>
+      </c>
+      <c r="D88" s="6"/>
+      <c r="E88" s="6"/>
+      <c r="F88" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="G88" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H88" s="9"/>
-      <c r="I88" s="9"/>
-      <c r="J88" s="9"/>
-      <c r="K88" s="9"/>
-      <c r="L88" s="9"/>
-      <c r="M88" s="9"/>
-      <c r="N88" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="H88" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="I88" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J88" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K88" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L88" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M88" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="N88" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="O88" s="8" t="n">
         <f aca="false">E88=""</f>
         <v>1</v>
       </c>
-      <c r="P88" s="9"/>
-    </row>
-    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A89" s="9" t="s">
-        <v>289</v>
+      <c r="P88" s="10"/>
+    </row>
+    <row r="89" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C89" s="6" t="s">
-        <v>290</v>
-      </c>
-      <c r="D89" s="9"/>
-      <c r="E89" s="9" t="s">
-        <v>291</v>
-      </c>
-      <c r="F89" s="11" t="s">
-        <v>115</v>
+        <v>267</v>
+      </c>
+      <c r="D89" s="6"/>
+      <c r="E89" s="6"/>
+      <c r="F89" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="G89" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H89" s="9"/>
-      <c r="I89" s="9"/>
-      <c r="J89" s="9"/>
-      <c r="K89" s="9"/>
-      <c r="L89" s="9"/>
-      <c r="M89" s="9"/>
-      <c r="N89" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="H89" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="I89" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J89" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K89" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L89" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M89" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="N89" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="O89" s="8" t="n">
         <f aca="false">E89=""</f>
-        <v>0</v>
-      </c>
-      <c r="P89" s="9"/>
-    </row>
-    <row r="90" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A90" s="9" t="s">
-        <v>291</v>
+        <v>1</v>
+      </c>
+      <c r="P89" s="10"/>
+    </row>
+    <row r="90" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="6" t="s">
+        <v>268</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>292</v>
-      </c>
-      <c r="D90" s="9"/>
-      <c r="E90" s="9"/>
-      <c r="F90" s="11" t="s">
-        <v>115</v>
+        <v>269</v>
+      </c>
+      <c r="D90" s="6"/>
+      <c r="E90" s="6"/>
+      <c r="F90" s="7" t="s">
+        <v>104</v>
       </c>
       <c r="G90" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H90" s="9"/>
-      <c r="I90" s="9"/>
-      <c r="J90" s="9"/>
-      <c r="K90" s="9"/>
-      <c r="L90" s="9"/>
-      <c r="M90" s="9"/>
-      <c r="N90" s="9"/>
+        <v>105</v>
+      </c>
+      <c r="H90" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="I90" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="J90" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="K90" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="L90" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="M90" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="N90" s="6" t="s">
+        <v>112</v>
+      </c>
       <c r="O90" s="8" t="n">
         <f aca="false">E90=""</f>
         <v>1</v>
       </c>
-      <c r="P90" s="9"/>
+      <c r="P90" s="10"/>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A91" s="9" t="s">
-        <v>293</v>
+      <c r="A91" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="B91" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>294</v>
-      </c>
-      <c r="D91" s="9"/>
-      <c r="E91" s="9" t="s">
-        <v>295</v>
-      </c>
-      <c r="F91" s="11" t="s">
-        <v>115</v>
+        <v>271</v>
+      </c>
+      <c r="D91" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E91" s="6"/>
+      <c r="F91" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="G91" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H91" s="9"/>
-      <c r="I91" s="9"/>
-      <c r="J91" s="9"/>
-      <c r="K91" s="9"/>
-      <c r="L91" s="9"/>
-      <c r="M91" s="9"/>
-      <c r="N91" s="9"/>
+      <c r="H91" s="6"/>
+      <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
+      <c r="M91" s="6"/>
+      <c r="N91" s="6"/>
       <c r="O91" s="8" t="n">
         <f aca="false">E91=""</f>
-        <v>0</v>
-      </c>
-      <c r="P91" s="9"/>
-    </row>
-    <row r="92" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A92" s="9" t="s">
-        <v>295</v>
+        <v>1</v>
+      </c>
+      <c r="P91" s="10"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="B92" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C92" s="6" t="s">
-        <v>296</v>
-      </c>
-      <c r="D92" s="9"/>
-      <c r="E92" s="9"/>
-      <c r="F92" s="11" t="s">
-        <v>115</v>
+        <v>273</v>
+      </c>
+      <c r="D92" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E92" s="6"/>
+      <c r="F92" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="G92" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H92" s="9"/>
-      <c r="I92" s="9"/>
-      <c r="J92" s="9"/>
-      <c r="K92" s="9"/>
-      <c r="L92" s="9"/>
-      <c r="M92" s="9"/>
-      <c r="N92" s="9"/>
+      <c r="H92" s="6"/>
+      <c r="I92" s="6"/>
+      <c r="J92" s="6"/>
+      <c r="K92" s="6"/>
+      <c r="L92" s="6"/>
+      <c r="M92" s="6"/>
+      <c r="N92" s="6"/>
       <c r="O92" s="8" t="n">
         <f aca="false">E92=""</f>
         <v>1</v>
       </c>
-      <c r="P92" s="9"/>
+      <c r="P92" s="10"/>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A93" s="9" t="s">
-        <v>297</v>
+      <c r="A93" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="B93" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C93" s="9" t="s">
-        <v>298</v>
-      </c>
-      <c r="D93" s="9"/>
-      <c r="E93" s="9" t="s">
-        <v>299</v>
-      </c>
-      <c r="F93" s="11" t="s">
-        <v>115</v>
+      <c r="C93" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="D93" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E93" s="6"/>
+      <c r="F93" s="7" t="s">
+        <v>143</v>
       </c>
       <c r="G93" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H93" s="9"/>
-      <c r="I93" s="9"/>
-      <c r="J93" s="9"/>
-      <c r="K93" s="9"/>
-      <c r="L93" s="9"/>
-      <c r="M93" s="9"/>
-      <c r="N93" s="9"/>
+      <c r="H93" s="6"/>
+      <c r="I93" s="6"/>
+      <c r="J93" s="6"/>
+      <c r="K93" s="6"/>
+      <c r="L93" s="6"/>
+      <c r="M93" s="6"/>
+      <c r="N93" s="6"/>
       <c r="O93" s="8" t="n">
         <f aca="false">E93=""</f>
-        <v>0</v>
-      </c>
-      <c r="P93" s="9"/>
-    </row>
-    <row r="94" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A94" s="9" t="s">
-        <v>299</v>
+        <v>1</v>
+      </c>
+      <c r="P93" s="10"/>
+    </row>
+    <row r="94" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="6" t="s">
+        <v>276</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C94" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="D94" s="9"/>
-      <c r="E94" s="9"/>
-      <c r="F94" s="11" t="s">
-        <v>115</v>
+        <v>277</v>
+      </c>
+      <c r="D94" s="6"/>
+      <c r="E94" s="6" t="s">
+        <v>138</v>
+      </c>
+      <c r="F94" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G94" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H94" s="9"/>
-      <c r="I94" s="9"/>
-      <c r="J94" s="9"/>
-      <c r="K94" s="9"/>
-      <c r="L94" s="9"/>
-      <c r="M94" s="9"/>
-      <c r="N94" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H94" s="6"/>
+      <c r="I94" s="6"/>
+      <c r="J94" s="6"/>
+      <c r="K94" s="6"/>
+      <c r="L94" s="6"/>
+      <c r="M94" s="6"/>
+      <c r="N94" s="6"/>
       <c r="O94" s="8" t="n">
         <f aca="false">E94=""</f>
-        <v>1</v>
-      </c>
-      <c r="P94" s="9"/>
-    </row>
-    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A95" s="9" t="s">
-        <v>301</v>
+        <v>0</v>
+      </c>
+      <c r="P94" s="10" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C95" s="9" t="s">
-        <v>302</v>
-      </c>
-      <c r="D95" s="9"/>
-      <c r="E95" s="9" t="s">
-        <v>303</v>
-      </c>
-      <c r="F95" s="11" t="s">
-        <v>115</v>
+        <v>33</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="D95" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="E95" s="6"/>
+      <c r="F95" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G95" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H95" s="9"/>
-      <c r="I95" s="9"/>
-      <c r="J95" s="9"/>
-      <c r="K95" s="9"/>
-      <c r="L95" s="9"/>
-      <c r="M95" s="9"/>
-      <c r="N95" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H95" s="6"/>
+      <c r="I95" s="6"/>
+      <c r="J95" s="6"/>
+      <c r="K95" s="6"/>
+      <c r="L95" s="6"/>
+      <c r="M95" s="6"/>
+      <c r="N95" s="6"/>
       <c r="O95" s="8" t="n">
         <f aca="false">E95=""</f>
-        <v>0</v>
-      </c>
-      <c r="P95" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="P95" s="10" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A96" s="9" t="s">
-        <v>303</v>
+      <c r="A96" s="6" t="s">
+        <v>283</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C96" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="D96" s="9"/>
-      <c r="E96" s="9"/>
-      <c r="F96" s="11" t="s">
-        <v>115</v>
+        <v>284</v>
+      </c>
+      <c r="D96" s="6"/>
+      <c r="E96" s="6" t="s">
+        <v>285</v>
+      </c>
+      <c r="F96" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G96" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H96" s="9"/>
-      <c r="I96" s="9"/>
-      <c r="J96" s="9"/>
-      <c r="K96" s="9"/>
-      <c r="L96" s="9"/>
-      <c r="M96" s="9"/>
-      <c r="N96" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H96" s="6"/>
+      <c r="I96" s="6"/>
+      <c r="J96" s="6"/>
+      <c r="K96" s="6"/>
+      <c r="L96" s="6"/>
+      <c r="M96" s="6"/>
+      <c r="N96" s="6"/>
       <c r="O96" s="8" t="n">
         <f aca="false">E96=""</f>
-        <v>1</v>
-      </c>
-      <c r="P96" s="9"/>
-    </row>
-    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A97" s="9" t="s">
-        <v>305</v>
+        <v>0</v>
+      </c>
+      <c r="P96" s="10" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="6" t="s">
+        <v>285</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C97" s="9" t="s">
-        <v>306</v>
-      </c>
-      <c r="D97" s="9"/>
-      <c r="E97" s="9" t="s">
-        <v>307</v>
-      </c>
-      <c r="F97" s="11" t="s">
-        <v>115</v>
+        <v>33</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>287</v>
+      </c>
+      <c r="D97" s="6" t="s">
+        <v>288</v>
+      </c>
+      <c r="E97" s="6"/>
+      <c r="F97" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G97" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H97" s="9"/>
-      <c r="I97" s="9"/>
-      <c r="J97" s="9"/>
-      <c r="K97" s="9"/>
-      <c r="L97" s="9"/>
-      <c r="M97" s="9"/>
-      <c r="N97" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H97" s="6"/>
+      <c r="I97" s="6"/>
+      <c r="J97" s="6"/>
+      <c r="K97" s="6"/>
+      <c r="L97" s="6"/>
+      <c r="M97" s="6"/>
+      <c r="N97" s="6"/>
       <c r="O97" s="8" t="n">
         <f aca="false">E97=""</f>
-        <v>0</v>
-      </c>
-      <c r="P97" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="P97" s="10" t="s">
+        <v>289</v>
+      </c>
     </row>
     <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A98" s="9" t="s">
-        <v>307</v>
+      <c r="A98" s="6" t="s">
+        <v>290</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C98" s="6" t="s">
-        <v>308</v>
-      </c>
-      <c r="D98" s="9"/>
-      <c r="E98" s="9"/>
-      <c r="F98" s="11" t="s">
-        <v>115</v>
+        <v>291</v>
+      </c>
+      <c r="D98" s="6"/>
+      <c r="E98" s="6" t="s">
+        <v>292</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G98" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H98" s="9"/>
-      <c r="I98" s="9"/>
-      <c r="J98" s="9"/>
-      <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
-      <c r="M98" s="9"/>
-      <c r="N98" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H98" s="6"/>
+      <c r="I98" s="6"/>
+      <c r="J98" s="6"/>
+      <c r="K98" s="6"/>
+      <c r="L98" s="6"/>
+      <c r="M98" s="6"/>
+      <c r="N98" s="6"/>
       <c r="O98" s="8" t="n">
         <f aca="false">E98=""</f>
-        <v>1</v>
-      </c>
-      <c r="P98" s="9"/>
-    </row>
-    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="9" t="s">
-        <v>309</v>
+        <v>0</v>
+      </c>
+      <c r="P98" s="10" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="6" t="s">
+        <v>292</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C99" s="9" t="s">
-        <v>310</v>
-      </c>
-      <c r="D99" s="9"/>
-      <c r="E99" s="9" t="s">
-        <v>311</v>
-      </c>
-      <c r="F99" s="11" t="s">
-        <v>115</v>
+        <v>33</v>
+      </c>
+      <c r="C99" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="D99" s="6" t="s">
+        <v>295</v>
+      </c>
+      <c r="E99" s="6"/>
+      <c r="F99" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G99" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H99" s="9"/>
-      <c r="I99" s="9"/>
-      <c r="J99" s="9"/>
-      <c r="K99" s="9"/>
-      <c r="L99" s="9"/>
-      <c r="M99" s="9"/>
-      <c r="N99" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H99" s="6"/>
+      <c r="I99" s="6"/>
+      <c r="J99" s="6"/>
+      <c r="K99" s="6"/>
+      <c r="L99" s="6"/>
+      <c r="M99" s="6"/>
+      <c r="N99" s="6"/>
       <c r="O99" s="8" t="n">
         <f aca="false">E99=""</f>
-        <v>0</v>
-      </c>
-      <c r="P99" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="P99" s="10" t="s">
+        <v>296</v>
+      </c>
     </row>
     <row r="100" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="9" t="s">
-        <v>311</v>
+      <c r="A100" s="6" t="s">
+        <v>297</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C100" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="D100" s="9"/>
-      <c r="E100" s="9"/>
-      <c r="F100" s="11" t="s">
-        <v>115</v>
+        <v>298</v>
+      </c>
+      <c r="D100" s="6"/>
+      <c r="E100" s="6" t="s">
+        <v>299</v>
+      </c>
+      <c r="F100" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G100" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H100" s="9"/>
-      <c r="I100" s="9"/>
-      <c r="J100" s="9"/>
-      <c r="K100" s="9"/>
-      <c r="L100" s="9"/>
-      <c r="M100" s="9"/>
-      <c r="N100" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H100" s="6"/>
+      <c r="I100" s="6"/>
+      <c r="J100" s="6"/>
+      <c r="K100" s="6"/>
+      <c r="L100" s="6"/>
+      <c r="M100" s="6"/>
+      <c r="N100" s="6"/>
       <c r="O100" s="8" t="n">
         <f aca="false">E100=""</f>
-        <v>1</v>
-      </c>
-      <c r="P100" s="9"/>
-    </row>
-    <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="9" t="s">
-        <v>313</v>
+        <v>0</v>
+      </c>
+      <c r="P100" s="10" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="101" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="6" t="s">
+        <v>299</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C101" s="9" t="s">
-        <v>314</v>
-      </c>
-      <c r="D101" s="9"/>
-      <c r="E101" s="9" t="s">
-        <v>315</v>
-      </c>
-      <c r="F101" s="11" t="s">
-        <v>115</v>
+        <v>33</v>
+      </c>
+      <c r="C101" s="6" t="s">
+        <v>301</v>
+      </c>
+      <c r="D101" s="6" t="s">
+        <v>302</v>
+      </c>
+      <c r="E101" s="6"/>
+      <c r="F101" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G101" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H101" s="9"/>
-      <c r="I101" s="9"/>
-      <c r="J101" s="9"/>
-      <c r="K101" s="9"/>
-      <c r="L101" s="9"/>
-      <c r="M101" s="9"/>
-      <c r="N101" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H101" s="6"/>
+      <c r="I101" s="6"/>
+      <c r="J101" s="6"/>
+      <c r="K101" s="6"/>
+      <c r="L101" s="6"/>
+      <c r="M101" s="6"/>
+      <c r="N101" s="6"/>
       <c r="O101" s="8" t="n">
         <f aca="false">E101=""</f>
-        <v>0</v>
-      </c>
-      <c r="P101" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="P101" s="10" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="9" t="s">
-        <v>315</v>
+      <c r="A102" s="6" t="s">
+        <v>304</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C102" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="D102" s="9"/>
-      <c r="E102" s="9"/>
-      <c r="F102" s="11" t="s">
-        <v>115</v>
+        <v>305</v>
+      </c>
+      <c r="D102" s="6"/>
+      <c r="E102" s="6" t="s">
+        <v>306</v>
+      </c>
+      <c r="F102" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G102" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H102" s="9"/>
-      <c r="I102" s="9"/>
-      <c r="J102" s="9"/>
-      <c r="K102" s="9"/>
-      <c r="L102" s="9"/>
-      <c r="M102" s="9"/>
-      <c r="N102" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H102" s="6"/>
+      <c r="I102" s="6"/>
+      <c r="J102" s="6"/>
+      <c r="K102" s="6"/>
+      <c r="L102" s="6"/>
+      <c r="M102" s="6"/>
+      <c r="N102" s="6"/>
       <c r="O102" s="8" t="n">
         <f aca="false">E102=""</f>
-        <v>1</v>
-      </c>
-      <c r="P102" s="9"/>
-    </row>
-    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="9" t="s">
-        <v>317</v>
+        <v>0</v>
+      </c>
+      <c r="P102" s="10" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="6" t="s">
+        <v>306</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C103" s="9" t="s">
-        <v>318</v>
-      </c>
-      <c r="D103" s="9"/>
-      <c r="E103" s="9" t="s">
-        <v>319</v>
-      </c>
-      <c r="F103" s="11" t="s">
-        <v>115</v>
+        <v>33</v>
+      </c>
+      <c r="C103" s="6" t="s">
+        <v>308</v>
+      </c>
+      <c r="D103" s="6" t="s">
+        <v>309</v>
+      </c>
+      <c r="E103" s="6"/>
+      <c r="F103" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G103" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H103" s="9"/>
-      <c r="I103" s="9"/>
-      <c r="J103" s="9"/>
-      <c r="K103" s="9"/>
-      <c r="L103" s="9"/>
-      <c r="M103" s="9"/>
-      <c r="N103" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H103" s="6"/>
+      <c r="I103" s="6"/>
+      <c r="J103" s="6"/>
+      <c r="K103" s="6"/>
+      <c r="L103" s="6"/>
+      <c r="M103" s="6"/>
+      <c r="N103" s="6"/>
       <c r="O103" s="8" t="n">
         <f aca="false">E103=""</f>
-        <v>0</v>
-      </c>
-      <c r="P103" s="9"/>
-    </row>
-    <row r="104" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="9" t="s">
-        <v>319</v>
+        <v>1</v>
+      </c>
+      <c r="P103" s="10" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="6" t="s">
+        <v>311</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="C104" s="6" t="s">
-        <v>320</v>
-      </c>
-      <c r="D104" s="9"/>
-      <c r="E104" s="9"/>
-      <c r="F104" s="11" t="s">
-        <v>115</v>
+        <v>312</v>
+      </c>
+      <c r="D104" s="6"/>
+      <c r="E104" s="6" t="s">
+        <v>313</v>
+      </c>
+      <c r="F104" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G104" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H104" s="9"/>
-      <c r="I104" s="9"/>
-      <c r="J104" s="9"/>
-      <c r="K104" s="9"/>
-      <c r="L104" s="9"/>
-      <c r="M104" s="9"/>
-      <c r="N104" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H104" s="6"/>
+      <c r="I104" s="6"/>
+      <c r="J104" s="6"/>
+      <c r="K104" s="6"/>
+      <c r="L104" s="6"/>
+      <c r="M104" s="6"/>
+      <c r="N104" s="6"/>
       <c r="O104" s="8" t="n">
         <f aca="false">E104=""</f>
-        <v>1</v>
-      </c>
-      <c r="P104" s="9"/>
-    </row>
-    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="9" t="s">
-        <v>321</v>
+        <v>0</v>
+      </c>
+      <c r="P104" s="10" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="105" customFormat="false" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="6" t="s">
+        <v>313</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C105" s="9" t="s">
-        <v>322</v>
-      </c>
-      <c r="D105" s="9"/>
-      <c r="E105" s="9" t="s">
-        <v>323</v>
-      </c>
-      <c r="F105" s="11" t="s">
-        <v>115</v>
+        <v>33</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>315</v>
+      </c>
+      <c r="D105" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="E105" s="6"/>
+      <c r="F105" s="7" t="s">
+        <v>139</v>
       </c>
       <c r="G105" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H105" s="9"/>
-      <c r="I105" s="9"/>
-      <c r="J105" s="9"/>
-      <c r="K105" s="9"/>
-      <c r="L105" s="9"/>
-      <c r="M105" s="9"/>
-      <c r="N105" s="9"/>
+        <v>278</v>
+      </c>
+      <c r="H105" s="6"/>
+      <c r="I105" s="6"/>
+      <c r="J105" s="6"/>
+      <c r="K105" s="6"/>
+      <c r="L105" s="6"/>
+      <c r="M105" s="6"/>
+      <c r="N105" s="6"/>
       <c r="O105" s="8" t="n">
         <f aca="false">E105=""</f>
-        <v>0</v>
-      </c>
-      <c r="P105" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="P105" s="10" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="106" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="9" t="s">
-        <v>323</v>
+      <c r="A106" s="6" t="s">
+        <v>318</v>
       </c>
       <c r="B106" s="6" t="s">
         <v>17</v>
       </c>
       <c r="C106" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="D106" s="9"/>
-      <c r="E106" s="9"/>
-      <c r="F106" s="11" t="s">
-        <v>115</v>
+        <v>319</v>
+      </c>
+      <c r="D106" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E106" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="F106" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="G106" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H106" s="9"/>
-      <c r="I106" s="9"/>
-      <c r="J106" s="9"/>
-      <c r="K106" s="9"/>
-      <c r="L106" s="9"/>
-      <c r="M106" s="9"/>
-      <c r="N106" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="H106" s="6"/>
+      <c r="I106" s="6"/>
+      <c r="J106" s="6"/>
+      <c r="K106" s="6"/>
+      <c r="L106" s="6"/>
+      <c r="M106" s="6"/>
+      <c r="N106" s="6"/>
       <c r="O106" s="8" t="n">
         <f aca="false">E106=""</f>
-        <v>1</v>
-      </c>
-      <c r="P106" s="9"/>
-    </row>
-    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="9" t="s">
-        <v>325</v>
+        <v>0</v>
+      </c>
+      <c r="P106" s="9" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="107" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="6" t="s">
+        <v>322</v>
       </c>
       <c r="B107" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C107" s="9" t="s">
-        <v>326</v>
-      </c>
-      <c r="D107" s="9"/>
-      <c r="E107" s="9" t="s">
-        <v>327</v>
-      </c>
-      <c r="F107" s="11" t="s">
-        <v>115</v>
+      <c r="C107" s="6" t="s">
+        <v>323</v>
+      </c>
+      <c r="D107" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E107" s="6" t="s">
+        <v>324</v>
+      </c>
+      <c r="F107" s="7" t="s">
+        <v>21</v>
       </c>
       <c r="G107" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H107" s="9"/>
-      <c r="I107" s="9"/>
-      <c r="J107" s="9"/>
-      <c r="K107" s="9"/>
-      <c r="L107" s="9"/>
-      <c r="M107" s="9"/>
-      <c r="N107" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="H107" s="6"/>
+      <c r="I107" s="6"/>
+      <c r="J107" s="6"/>
+      <c r="K107" s="6"/>
+      <c r="L107" s="6"/>
+      <c r="M107" s="6"/>
+      <c r="N107" s="6"/>
       <c r="O107" s="8" t="n">
         <f aca="false">E107=""</f>
         <v>0</v>
       </c>
-      <c r="P107" s="9"/>
-    </row>
-    <row r="108" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="9" t="s">
+      <c r="P107" s="9" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="108" customFormat="false" ht="113.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A108" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="B108" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="C108" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="B108" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C108" s="6" t="s">
-        <v>328</v>
-      </c>
-      <c r="D108" s="9"/>
-      <c r="E108" s="9"/>
-      <c r="F108" s="11" t="s">
-        <v>115</v>
+      <c r="D108" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="E108" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="G108" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="H108" s="9"/>
-      <c r="I108" s="9"/>
-      <c r="J108" s="9"/>
-      <c r="K108" s="9"/>
-      <c r="L108" s="9"/>
-      <c r="M108" s="9"/>
-      <c r="N108" s="9"/>
+      <c r="H108" s="6"/>
+      <c r="I108" s="6"/>
+      <c r="J108" s="6"/>
+      <c r="K108" s="6"/>
+      <c r="L108" s="6"/>
+      <c r="M108" s="6"/>
+      <c r="N108" s="6"/>
       <c r="O108" s="8" t="n">
         <f aca="false">E108=""</f>
-        <v>1</v>
-      </c>
-      <c r="P108" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="P108" s="9" t="s">
+        <v>328</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:P86"/>

</xml_diff>

<commit_message>
* korekta wielkiej literówki w 0.9.3, gdzie zmienne PM_coś_S/PM_coś_N miały w mianowniku NM_S/NM_N zamiast NM_X_S/NM_X_N * korekta wyliczania zmiennych PM_X_S i PM_X_N (te dwie wyjątkowo powinny mieć w mianowniku LEN zamiast NM_X_S i NM_X_N) * dodanie funkcji oblicz_pkd() wyliczającej zmienne opisujące PKD     * pozostawienie zmiennej "pkd" w przygotuj_zus_zdau()     * dodanie dołączania zbioru pkd do danych miesięcznych i kwartalnych w winietce generowania danych * wydzielenie funkcji przygotuj_zdu1() z przygotuj_zus(), aby można było łatwo dołączyć informację o płci oraz roku urodzenia * dodanie funkcji generuj_wartosci() używanej przy generowaniu raportów oraz wykorzystującej je winietki
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="zmienne" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="schemat" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="nauka" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">zmienne!$A$1:$S$278</definedName>
@@ -17,29 +18,29 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">zmienne!$A$1:$S$278</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">zmienne!$A$1:$S$278</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">zmienne!$A$1:$S$278</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">zmienne!$A$1:$Q$278</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$238</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0" vbProcedure="false">zmienne!$A$1:$S$278</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$S$278</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$Q$278</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$238</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$Q$278</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$238</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$Q$224</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$Q$278</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$238</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$Q$224</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$Q$224</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$223</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
@@ -51,6 +52,8 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">zmienne!$A$1:$P$160</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -62,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2014" uniqueCount="878">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2033" uniqueCount="878">
   <si>
     <t xml:space="preserve">zmienna</t>
   </si>
@@ -1552,7 +1555,7 @@
     <t xml:space="preserve">PM_X_S</t>
   </si>
   <si>
-    <t xml:space="preserve">100 * NM_X_S / NM_X_S</t>
+    <t xml:space="preserve">100 * NM_X_S / LEN</t>
   </si>
   <si>
     <t xml:space="preserve">STUDPROC</t>
@@ -1561,7 +1564,7 @@
     <t xml:space="preserve">PM_X_N</t>
   </si>
   <si>
-    <t xml:space="preserve">100 * NM_X_N / NM_X_N</t>
+    <t xml:space="preserve">100 * NM_X_N / LEN</t>
   </si>
   <si>
     <t xml:space="preserve">Identyfikator powiatu zamieszkania na koniec danego okresu
@@ -2110,6 +2113,300 @@
     <t xml:space="preserve">PM_B_N, PPOW_B_N</t>
   </si>
   <si>
+    <t xml:space="preserve">1. człon – rodzaj zmiennej</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2. człon – sytuacja na rynku pracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3. człon – studiowanie/kariera naukowa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4. człon – okienko czasu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dla miesięcy, w których studiował (wszystko jedno, czy na tym samym, czy innym kierunku studiów)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-ty rok przed uzyskaniu dyplomu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procent miesięcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">samoz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dla miesięcy, w których nie studiował na żadnym kierunku studiów</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Px</t>
+  </si>
+  <si>
+    <t xml:space="preserve">x-ty rok po uzyskaniem dyplomu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">suma zarobków</t>
+  </si>
+  <si>
+    <t xml:space="preserve">netat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dla miesięcy, w których studiował na danym (identyfikowanym przez ID_ZDAU) kierunku studiów – implikuje bycie stałą!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[brak]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okres od 1 miesiąca po uzyskaniu dyplomu do końca badanego okresu lub stała</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">średnie zarobki</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etat/netat/samoz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dla miesięcy przed rozpoczęciem danego (identyfikowanego przez ID_ZDAU) kierunku studiów – implikuje bycie stałą!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba miesięcy do uzyskania pierwszej pracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Z</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etat/netat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dla miesięcy, w których studiował – implikuje bycie stałą!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba utrat pracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etat/samoz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SLIC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okres ukończonych jako pierwsze studiów licencjackich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">IF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">należenie do pewnej podzbiorowości, np. IF_E – czy pracował na etacie, IF_ST czy był studentem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BD</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brak danych ZUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SMGR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okres ukończonych jako pierwsze studiów magisterskich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba pracodawców</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">macierzyński/tacierzyński</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SDR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okres ukończonych jako pierwsze studiów doktoranckich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NPN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">liczba nowych pracodawców</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mundurowy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okres od uzyskania pierwszego tytułu doktora do uzyskania pierwszego tytułu doktora habilitowanego</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">średnia liczba pracodawców</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sędzia, itp.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HAB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okres od uzyskania pierwszego tytułu doktora habilitowanego do uzyskania tytułu profesora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">procent pracodawców</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bezrobocie wliczając brak danych ZUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">okres od uzyskania tytułu profesora</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EPM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">średnia liczba pracodawco-miesięcy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bezrobocie pomijając braki danych ZUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENPN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">średnia liczba nowych pracodawców (w przeliczeniu na 12 miesięcy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inny tytuł ubezpieczenia ZUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ENUP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">średnia liczba utrat pracy (w przeliczeniu na 12 miesięcy)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bez etat/netat/samoz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bez etatu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">student</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dowolna</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etat/netat w nauce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etat w nauce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZNPN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etat/netat jednocześnie w nauce i poza nauką</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ZPN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">etat/netat poza nauką</t>
+  </si>
+  <si>
     <t xml:space="preserve">ETAP</t>
   </si>
   <si>
@@ -2120,24 +2417,6 @@
   </si>
   <si>
     <t xml:space="preserve">pozostałe</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SLIC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SMGR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SDR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HAB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROF</t>
   </si>
   <si>
     <t xml:space="preserve">DATA_OD</t>
@@ -2495,9 +2774,6 @@
     <t xml:space="preserve">A</t>
   </si>
   <si>
-    <t xml:space="preserve">S</t>
-  </si>
-  <si>
     <t xml:space="preserve">CUDZOZIEMIEC</t>
   </si>
   <si>
@@ -2507,9 +2783,6 @@
     <t xml:space="preserve">studia stacjonarne/niestacjonarne</t>
   </si>
   <si>
-    <t xml:space="preserve">N</t>
-  </si>
-  <si>
     <t xml:space="preserve">POZIOM</t>
   </si>
   <si>
@@ -2529,276 +2802,6 @@
   </si>
   <si>
     <t xml:space="preserve">ROK_UR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1. człon – rodzaj zmiennej</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2. człon – sytuacja na rynku pracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">3. człon – studiowanie/kariera naukowa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4. człon – okienko czasu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dla miesięcy, w których studiował (wszystko jedno, czy na tym samym, czy innym kierunku studiów)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x-ty rok przed uzyskaniu dyplomu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procent miesięcy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">samoz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dla miesięcy, w których nie studiował na żadnym kierunku studiów</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Px</t>
-  </si>
-  <si>
-    <t xml:space="preserve">x-ty rok po uzyskaniem dyplomu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">suma zarobków</t>
-  </si>
-  <si>
-    <t xml:space="preserve">netat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dla miesięcy, w których studiował na danym (identyfikowanym przez ID_ZDAU) kierunku studiów – implikuje bycie stałą!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[brak]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">okres od 1 miesiąca po uzyskaniu dyplomu do końca badanego okresu lub stała</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EZ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">średnie zarobki</t>
-  </si>
-  <si>
-    <t xml:space="preserve">P</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etat/netat/samoz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dla miesięcy przed rozpoczęciem danego (identyfikowanego przez ID_ZDAU) kierunku studiów – implikuje bycie stałą!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba miesięcy do uzyskania pierwszej pracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Z</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etat/netat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ST</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dla miesięcy, w których studiował – implikuje bycie stałą!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba utrat pracy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ES</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etat/samoz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">okres ukończonych jako pierwsze studiów licencjackich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">należenie do pewnej podzbiorowości, np. IF_E – czy pracował na etacie, IF_ST czy był studentem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brak danych ZUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">okres ukończonych jako pierwsze studiów magisterskich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba pracodawców</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">macierzyński/tacierzyński</t>
-  </si>
-  <si>
-    <t xml:space="preserve">okres ukończonych jako pierwsze studiów doktoranckich</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NPN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">liczba nowych pracodawców</t>
-  </si>
-  <si>
-    <t xml:space="preserve">M</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mundurowy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">okres od uzyskania pierwszego tytułu doktora do uzyskania pierwszego tytułu doktora habilitowanego</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">średnia liczba pracodawców</t>
-  </si>
-  <si>
-    <t xml:space="preserve">J</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sędzia, itp.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">okres od uzyskania pierwszego tytułu doktora habilitowanego do uzyskania tytułu profesora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">procent pracodawców</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bezrobocie wliczając brak danych ZUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">okres od uzyskania tytułu profesora</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EPM</t>
-  </si>
-  <si>
-    <t xml:space="preserve">średnia liczba pracodawco-miesięcy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">B2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bezrobocie pomijając braki danych ZUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENPN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">średnia liczba nowych pracodawców (w przeliczeniu na 12 miesięcy)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inny tytuł ubezpieczenia ZUS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ENUP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">średnia liczba utrat pracy (w przeliczeniu na 12 miesięcy)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BP</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bez etat/netat/samoz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">bez etatu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">student</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dowolna</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etat/netat w nauce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etat w nauce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZNPN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etat/netat jednocześnie w nauce i poza nauką</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ZPN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">etat/netat poza nauką</t>
   </si>
 </sst>
 </file>
@@ -3168,6 +3171,18 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="12" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3181,18 +3196,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="13" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="13" fillId="8" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -3293,12 +3296,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMH296"/>
+  <dimension ref="A1:AMH224"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F210" activeCellId="0" sqref="F210"/>
+      <selection pane="bottomLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6160,7 +6163,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
         <v>103</v>
       </c>
@@ -14161,7 +14164,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="157" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="157" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A157" s="10" t="s">
         <v>476</v>
       </c>
@@ -16638,1157 +16641,6 @@
         <v>646</v>
       </c>
       <c r="Q224" s="7"/>
-    </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A225" s="1" t="s">
-        <v>650</v>
-      </c>
-      <c r="B225" s="1" t="s">
-        <v>651</v>
-      </c>
-      <c r="C225" s="1" t="s">
-        <v>652</v>
-      </c>
-      <c r="F225" s="0"/>
-      <c r="H225" s="1" t="s">
-        <v>653</v>
-      </c>
-      <c r="I225" s="1" t="s">
-        <v>654</v>
-      </c>
-      <c r="J225" s="1" t="s">
-        <v>655</v>
-      </c>
-      <c r="K225" s="1" t="s">
-        <v>656</v>
-      </c>
-      <c r="L225" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="M225" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="N225" s="1" t="s">
-        <v>659</v>
-      </c>
-      <c r="R225" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A226" s="14" t="s">
-        <v>660</v>
-      </c>
-      <c r="B226" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C226" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="F226" s="2" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A227" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="B227" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C227" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="F227" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="R227" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A228" s="0" t="s">
-        <v>665</v>
-      </c>
-      <c r="B228" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C228" s="1" t="s">
-        <v>662</v>
-      </c>
-      <c r="F228" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="R228" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A229" s="14" t="s">
-        <v>666</v>
-      </c>
-      <c r="B229" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C229" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="F229" s="2" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A230" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="B230" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C230" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="F230" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="R230" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A231" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="B231" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C231" s="1" t="s">
-        <v>667</v>
-      </c>
-      <c r="F231" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="R231" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A232" s="14" t="s">
-        <v>670</v>
-      </c>
-      <c r="B232" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C232" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="F232" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="R232" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A233" s="1" t="s">
-        <v>672</v>
-      </c>
-      <c r="B233" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C233" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="F233" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="R233" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A234" s="1" t="s">
-        <v>673</v>
-      </c>
-      <c r="B234" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C234" s="1" t="s">
-        <v>674</v>
-      </c>
-      <c r="F234" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="R234" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A235" s="1" t="s">
-        <v>675</v>
-      </c>
-      <c r="B235" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C235" s="1" t="s">
-        <v>676</v>
-      </c>
-      <c r="F235" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="R235" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A236" s="1" t="s">
-        <v>677</v>
-      </c>
-      <c r="B236" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C236" s="1" t="s">
-        <v>678</v>
-      </c>
-      <c r="F236" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="R236" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A237" s="14" t="s">
-        <v>679</v>
-      </c>
-      <c r="B237" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C237" s="1" t="s">
-        <v>680</v>
-      </c>
-      <c r="F237" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="R237" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A238" s="1" t="s">
-        <v>681</v>
-      </c>
-      <c r="B238" s="1" t="s">
-        <v>661</v>
-      </c>
-      <c r="C238" s="1" t="s">
-        <v>682</v>
-      </c>
-      <c r="F238" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="H238" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="I238" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="Q238" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="R238" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="239" customFormat="false" ht="35.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A239" s="14" t="s">
-        <v>684</v>
-      </c>
-      <c r="B239" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C239" s="15" t="s">
-        <v>685</v>
-      </c>
-      <c r="D239" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="E239" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="F239" s="2" t="s">
-        <v>687</v>
-      </c>
-      <c r="Q239" s="0"/>
-    </row>
-    <row r="240" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A240" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="B240" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C240" s="15" t="s">
-        <v>689</v>
-      </c>
-      <c r="D240" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="E240" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="F240" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="R240" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="241" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A241" s="1" t="s">
-        <v>690</v>
-      </c>
-      <c r="B241" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C241" s="15" t="s">
-        <v>689</v>
-      </c>
-      <c r="D241" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="E241" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="F241" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="R241" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="242" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A242" s="1" t="s">
-        <v>691</v>
-      </c>
-      <c r="B242" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C242" s="15" t="s">
-        <v>692</v>
-      </c>
-      <c r="D242" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="F242" s="2" t="s">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A243" s="1" t="s">
-        <v>693</v>
-      </c>
-      <c r="B243" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C243" s="1" t="s">
-        <v>694</v>
-      </c>
-      <c r="F243" s="2" t="s">
-        <v>663</v>
-      </c>
-      <c r="Q243" s="16" t="s">
-        <v>695</v>
-      </c>
-      <c r="R243" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A244" s="16" t="s">
-        <v>696</v>
-      </c>
-      <c r="B244" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C244" s="16" t="s">
-        <v>697</v>
-      </c>
-      <c r="D244" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="F244" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q244" s="0"/>
-      <c r="R244" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A245" s="16" t="s">
-        <v>698</v>
-      </c>
-      <c r="B245" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="C245" s="16" t="s">
-        <v>699</v>
-      </c>
-      <c r="D245" s="1" t="s">
-        <v>686</v>
-      </c>
-      <c r="F245" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="Q245" s="0"/>
-      <c r="R245" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A246" s="1" t="s">
-        <v>700</v>
-      </c>
-      <c r="B246" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C246" s="1" t="s">
-        <v>701</v>
-      </c>
-      <c r="R246" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A247" s="1" t="s">
-        <v>702</v>
-      </c>
-      <c r="B247" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C247" s="0" t="s">
-        <v>703</v>
-      </c>
-      <c r="R247" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A248" s="1" t="s">
-        <v>704</v>
-      </c>
-      <c r="B248" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C248" s="1" t="s">
-        <v>705</v>
-      </c>
-      <c r="R248" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A249" s="1" t="s">
-        <v>706</v>
-      </c>
-      <c r="B249" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C249" s="1" t="s">
-        <v>707</v>
-      </c>
-      <c r="R249" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A250" s="1" t="s">
-        <v>708</v>
-      </c>
-      <c r="B250" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C250" s="1" t="s">
-        <v>709</v>
-      </c>
-      <c r="R250" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A251" s="1" t="s">
-        <v>710</v>
-      </c>
-      <c r="B251" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C251" s="1" t="s">
-        <v>711</v>
-      </c>
-      <c r="R251" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A252" s="1" t="s">
-        <v>712</v>
-      </c>
-      <c r="B252" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C252" s="1" t="s">
-        <v>713</v>
-      </c>
-      <c r="D252" s="0"/>
-      <c r="E252" s="0"/>
-      <c r="R252" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A253" s="1" t="s">
-        <v>714</v>
-      </c>
-      <c r="B253" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C253" s="1" t="s">
-        <v>715</v>
-      </c>
-      <c r="D253" s="0"/>
-      <c r="E253" s="0"/>
-      <c r="R253" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A254" s="1" t="s">
-        <v>716</v>
-      </c>
-      <c r="B254" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C254" s="1" t="s">
-        <v>717</v>
-      </c>
-      <c r="D254" s="0"/>
-      <c r="E254" s="0"/>
-      <c r="R254" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A255" s="1" t="s">
-        <v>718</v>
-      </c>
-      <c r="B255" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C255" s="1" t="s">
-        <v>719</v>
-      </c>
-      <c r="D255" s="0"/>
-      <c r="E255" s="0"/>
-      <c r="R255" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A256" s="1" t="s">
-        <v>720</v>
-      </c>
-      <c r="B256" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C256" s="1" t="s">
-        <v>721</v>
-      </c>
-      <c r="D256" s="0"/>
-      <c r="E256" s="0"/>
-      <c r="R256" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A257" s="1" t="s">
-        <v>722</v>
-      </c>
-      <c r="B257" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C257" s="1" t="s">
-        <v>723</v>
-      </c>
-      <c r="D257" s="0"/>
-      <c r="E257" s="0"/>
-      <c r="R257" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="258" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A258" s="1" t="s">
-        <v>724</v>
-      </c>
-      <c r="B258" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C258" s="15" t="s">
-        <v>725</v>
-      </c>
-      <c r="R258" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A259" s="1" t="s">
-        <v>726</v>
-      </c>
-      <c r="B259" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C259" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="E259" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="R259" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A260" s="1" t="s">
-        <v>729</v>
-      </c>
-      <c r="B260" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C260" s="1" t="s">
-        <v>730</v>
-      </c>
-      <c r="E260" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="R260" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A261" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="B261" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C261" s="1" t="s">
-        <v>732</v>
-      </c>
-      <c r="R261" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A262" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="B262" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C262" s="1" t="s">
-        <v>733</v>
-      </c>
-      <c r="R262" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A263" s="1" t="s">
-        <v>734</v>
-      </c>
-      <c r="B263" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C263" s="1" t="s">
-        <v>735</v>
-      </c>
-      <c r="E263" s="1" t="s">
-        <v>728</v>
-      </c>
-      <c r="R263" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A264" s="1" t="s">
-        <v>736</v>
-      </c>
-      <c r="B264" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C264" s="1" t="s">
-        <v>737</v>
-      </c>
-      <c r="E264" s="1" t="s">
-        <v>731</v>
-      </c>
-      <c r="R264" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A265" s="1" t="s">
-        <v>738</v>
-      </c>
-      <c r="B265" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C265" s="1" t="s">
-        <v>739</v>
-      </c>
-      <c r="E265" s="1" t="s">
-        <v>740</v>
-      </c>
-      <c r="R265" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A266" s="1" t="s">
-        <v>741</v>
-      </c>
-      <c r="B266" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C266" s="1" t="s">
-        <v>742</v>
-      </c>
-      <c r="E266" s="1" t="s">
-        <v>743</v>
-      </c>
-      <c r="R266" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A267" s="1" t="s">
-        <v>744</v>
-      </c>
-      <c r="B267" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C267" s="1" t="s">
-        <v>745</v>
-      </c>
-      <c r="R267" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A268" s="1" t="s">
-        <v>746</v>
-      </c>
-      <c r="B268" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C268" s="1" t="s">
-        <v>747</v>
-      </c>
-      <c r="R268" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="269" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A269" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="B269" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C269" s="1" t="s">
-        <v>749</v>
-      </c>
-      <c r="R269" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="270" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A270" s="1" t="s">
-        <v>750</v>
-      </c>
-      <c r="B270" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C270" s="1" t="s">
-        <v>751</v>
-      </c>
-      <c r="R270" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="271" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A271" s="1" t="s">
-        <v>752</v>
-      </c>
-      <c r="B271" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C271" s="1" t="s">
-        <v>753</v>
-      </c>
-      <c r="R271" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="272" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A272" s="1" t="s">
-        <v>754</v>
-      </c>
-      <c r="B272" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C272" s="1" t="s">
-        <v>755</v>
-      </c>
-      <c r="R272" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="273" customFormat="false" ht="57.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A273" s="1" t="s">
-        <v>756</v>
-      </c>
-      <c r="B273" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C273" s="1" t="s">
-        <v>757</v>
-      </c>
-      <c r="Q273" s="17" t="s">
-        <v>758</v>
-      </c>
-      <c r="R273" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="274" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A274" s="1" t="s">
-        <v>759</v>
-      </c>
-      <c r="B274" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C274" s="1" t="s">
-        <v>760</v>
-      </c>
-      <c r="E274" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="R274" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="275" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A275" s="1" t="s">
-        <v>762</v>
-      </c>
-      <c r="B275" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C275" s="1" t="s">
-        <v>763</v>
-      </c>
-      <c r="E275" s="1" t="s">
-        <v>761</v>
-      </c>
-      <c r="R275" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="276" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A276" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="B276" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C276" s="1" t="s">
-        <v>765</v>
-      </c>
-      <c r="R276" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="277" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A277" s="1" t="s">
-        <v>766</v>
-      </c>
-      <c r="B277" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C277" s="1" t="s">
-        <v>767</v>
-      </c>
-      <c r="E277" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="R277" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="278" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A278" s="1" t="s">
-        <v>768</v>
-      </c>
-      <c r="B278" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="C278" s="1" t="s">
-        <v>769</v>
-      </c>
-      <c r="E278" s="1" t="s">
-        <v>764</v>
-      </c>
-      <c r="R278" s="1" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="280" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A280" s="1" t="s">
-        <v>770</v>
-      </c>
-      <c r="B280" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F280" s="2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="281" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A281" s="1" t="s">
-        <v>771</v>
-      </c>
-      <c r="B281" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F281" s="2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="282" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A282" s="1" t="s">
-        <v>772</v>
-      </c>
-      <c r="B282" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F282" s="2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="283" customFormat="false" ht="23.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A283" s="1" t="s">
-        <v>773</v>
-      </c>
-      <c r="B283" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C283" s="15" t="s">
-        <v>774</v>
-      </c>
-      <c r="F283" s="2" t="s">
-        <v>687</v>
-      </c>
-      <c r="H283" s="1" t="s">
-        <v>775</v>
-      </c>
-      <c r="I283" s="1" t="s">
-        <v>776</v>
-      </c>
-    </row>
-    <row r="284" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A284" s="1" t="s">
-        <v>777</v>
-      </c>
-      <c r="B284" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F284" s="2" t="s">
-        <v>687</v>
-      </c>
-      <c r="H284" s="1" t="s">
-        <v>241</v>
-      </c>
-      <c r="I284" s="1" t="s">
-        <v>242</v>
-      </c>
-    </row>
-    <row r="285" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A285" s="1" t="s">
-        <v>679</v>
-      </c>
-      <c r="B285" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F285" s="2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="286" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A286" s="1" t="s">
-        <v>778</v>
-      </c>
-      <c r="B286" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C286" s="1" t="s">
-        <v>779</v>
-      </c>
-      <c r="F286" s="2" t="s">
-        <v>687</v>
-      </c>
-      <c r="H286" s="1" t="s">
-        <v>776</v>
-      </c>
-      <c r="I286" s="1" t="s">
-        <v>780</v>
-      </c>
-    </row>
-    <row r="287" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A287" s="1" t="s">
-        <v>781</v>
-      </c>
-      <c r="B287" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C287" s="1" t="s">
-        <v>782</v>
-      </c>
-      <c r="F287" s="2" t="s">
-        <v>687</v>
-      </c>
-      <c r="H287" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="I287" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J287" s="1" t="s">
-        <v>783</v>
-      </c>
-      <c r="K287" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="L287" s="1" t="s">
-        <v>657</v>
-      </c>
-      <c r="M287" s="1" t="s">
-        <v>658</v>
-      </c>
-      <c r="N287" s="1" t="s">
-        <v>659</v>
-      </c>
-    </row>
-    <row r="288" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A288" s="1" t="s">
-        <v>784</v>
-      </c>
-      <c r="B288" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="C288" s="1" t="s">
-        <v>785</v>
-      </c>
-      <c r="F288" s="2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="289" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A289" s="1" t="s">
-        <v>664</v>
-      </c>
-      <c r="B289" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F289" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="290" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A290" s="1" t="s">
-        <v>665</v>
-      </c>
-      <c r="B290" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F290" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="291" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A291" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="B291" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F291" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="292" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A292" s="1" t="s">
-        <v>669</v>
-      </c>
-      <c r="B292" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F292" s="2" t="s">
-        <v>286</v>
-      </c>
-    </row>
-    <row r="293" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A293" s="1" t="s">
-        <v>660</v>
-      </c>
-      <c r="B293" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F293" s="2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="294" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A294" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="B294" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F294" s="2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="295" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A295" s="1" t="s">
-        <v>786</v>
-      </c>
-      <c r="B295" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F295" s="2" t="s">
-        <v>687</v>
-      </c>
-    </row>
-    <row r="296" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A296" s="1" t="s">
-        <v>787</v>
-      </c>
-      <c r="B296" s="1" t="s">
-        <v>273</v>
-      </c>
-      <c r="F296" s="2" t="s">
-        <v>687</v>
-      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:S278"/>
@@ -17813,7 +16665,7 @@
   </sheetPr>
   <dimension ref="A1:L22"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E6" activeCellId="0" sqref="E6"/>
     </sheetView>
   </sheetViews>
@@ -17831,463 +16683,463 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="18" t="s">
-        <v>788</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19"/>
-      <c r="D1" s="18" t="s">
-        <v>789</v>
-      </c>
-      <c r="E1" s="18"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="18" t="s">
-        <v>790</v>
-      </c>
-      <c r="H1" s="18"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="18" t="s">
-        <v>791</v>
-      </c>
-      <c r="K1" s="18"/>
-      <c r="L1" s="19"/>
+      <c r="A1" s="14" t="s">
+        <v>650</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="14" t="s">
+        <v>651</v>
+      </c>
+      <c r="E1" s="14"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="14" t="s">
+        <v>652</v>
+      </c>
+      <c r="H1" s="14"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="14" t="s">
+        <v>653</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="15"/>
     </row>
     <row r="2" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
-        <v>792</v>
+        <v>654</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>793</v>
-      </c>
-      <c r="C2" s="19"/>
+        <v>655</v>
+      </c>
+      <c r="C2" s="15"/>
       <c r="D2" s="10" t="s">
-        <v>794</v>
+        <v>656</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>795</v>
-      </c>
-      <c r="F2" s="19"/>
+        <v>657</v>
+      </c>
+      <c r="F2" s="15"/>
       <c r="G2" s="10" t="s">
-        <v>776</v>
+        <v>658</v>
       </c>
       <c r="H2" s="10" t="s">
-        <v>796</v>
-      </c>
-      <c r="I2" s="19"/>
+        <v>659</v>
+      </c>
+      <c r="I2" s="15"/>
       <c r="J2" s="10" t="s">
-        <v>797</v>
+        <v>660</v>
       </c>
       <c r="K2" s="10" t="s">
-        <v>798</v>
-      </c>
-      <c r="L2" s="19"/>
+        <v>661</v>
+      </c>
+      <c r="L2" s="15"/>
     </row>
     <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
-        <v>799</v>
+        <v>662</v>
       </c>
       <c r="B3" s="10" t="s">
-        <v>800</v>
-      </c>
-      <c r="C3" s="19"/>
+        <v>663</v>
+      </c>
+      <c r="C3" s="15"/>
       <c r="D3" s="10" t="s">
-        <v>776</v>
+        <v>658</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>801</v>
-      </c>
-      <c r="F3" s="19"/>
+        <v>664</v>
+      </c>
+      <c r="F3" s="15"/>
       <c r="G3" s="10" t="s">
-        <v>780</v>
+        <v>665</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>802</v>
-      </c>
-      <c r="I3" s="19"/>
+        <v>666</v>
+      </c>
+      <c r="I3" s="15"/>
       <c r="J3" s="10" t="s">
-        <v>803</v>
+        <v>667</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>804</v>
-      </c>
-      <c r="L3" s="19"/>
+        <v>668</v>
+      </c>
+      <c r="L3" s="15"/>
     </row>
     <row r="4" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>134</v>
       </c>
       <c r="B4" s="10" t="s">
-        <v>805</v>
-      </c>
-      <c r="C4" s="19"/>
+        <v>669</v>
+      </c>
+      <c r="C4" s="15"/>
       <c r="D4" s="10" t="s">
-        <v>780</v>
+        <v>665</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>806</v>
-      </c>
-      <c r="F4" s="19"/>
+        <v>670</v>
+      </c>
+      <c r="F4" s="15"/>
       <c r="G4" s="10" t="s">
-        <v>807</v>
+        <v>671</v>
       </c>
       <c r="H4" s="10" t="s">
-        <v>808</v>
-      </c>
-      <c r="I4" s="19"/>
+        <v>672</v>
+      </c>
+      <c r="I4" s="15"/>
       <c r="J4" s="10" t="s">
-        <v>809</v>
+        <v>673</v>
       </c>
       <c r="K4" s="10" t="s">
-        <v>810</v>
-      </c>
-      <c r="L4" s="19"/>
+        <v>674</v>
+      </c>
+      <c r="L4" s="15"/>
     </row>
     <row r="5" customFormat="false" ht="68.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
-        <v>811</v>
+        <v>675</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>812</v>
-      </c>
-      <c r="C5" s="19"/>
+        <v>676</v>
+      </c>
+      <c r="C5" s="15"/>
       <c r="D5" s="10" t="s">
-        <v>813</v>
+        <v>677</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>814</v>
-      </c>
-      <c r="F5" s="19"/>
+        <v>678</v>
+      </c>
+      <c r="F5" s="15"/>
       <c r="G5" s="10" t="s">
-        <v>815</v>
+        <v>679</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>816</v>
-      </c>
-      <c r="I5" s="19"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="19"/>
-    </row>
-    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>680</v>
+      </c>
+      <c r="I5" s="15"/>
+      <c r="J5" s="16"/>
+      <c r="K5" s="16"/>
+      <c r="L5" s="15"/>
+    </row>
+    <row r="6" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
-        <v>817</v>
+        <v>681</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>818</v>
-      </c>
-      <c r="C6" s="19"/>
+        <v>682</v>
+      </c>
+      <c r="C6" s="15"/>
       <c r="D6" s="10" t="s">
-        <v>819</v>
+        <v>683</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>820</v>
-      </c>
-      <c r="F6" s="19"/>
+        <v>684</v>
+      </c>
+      <c r="F6" s="15"/>
       <c r="G6" s="10" t="s">
-        <v>821</v>
+        <v>685</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>822</v>
-      </c>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
+        <v>686</v>
+      </c>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
     </row>
     <row r="7" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
-        <v>823</v>
+        <v>687</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>824</v>
-      </c>
-      <c r="C7" s="19"/>
+        <v>688</v>
+      </c>
+      <c r="C7" s="15"/>
       <c r="D7" s="7" t="s">
-        <v>825</v>
+        <v>689</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>826</v>
-      </c>
-      <c r="F7" s="19"/>
+        <v>690</v>
+      </c>
+      <c r="F7" s="15"/>
       <c r="G7" s="10" t="s">
-        <v>654</v>
+        <v>691</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>827</v>
-      </c>
-      <c r="I7" s="19"/>
-      <c r="L7" s="19"/>
+        <v>692</v>
+      </c>
+      <c r="I7" s="15"/>
+      <c r="L7" s="15"/>
     </row>
     <row r="8" customFormat="false" ht="40.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
-        <v>828</v>
+        <v>693</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>829</v>
-      </c>
-      <c r="C8" s="19"/>
+        <v>694</v>
+      </c>
+      <c r="C8" s="15"/>
       <c r="D8" s="10" t="s">
-        <v>830</v>
+        <v>695</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>831</v>
-      </c>
-      <c r="F8" s="19"/>
+        <v>696</v>
+      </c>
+      <c r="F8" s="15"/>
       <c r="G8" s="10" t="s">
-        <v>655</v>
+        <v>697</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>832</v>
-      </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
+        <v>698</v>
+      </c>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
     </row>
     <row r="9" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
-        <v>833</v>
+        <v>699</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>834</v>
-      </c>
-      <c r="C9" s="19"/>
+        <v>700</v>
+      </c>
+      <c r="C9" s="15"/>
       <c r="D9" s="10" t="s">
-        <v>835</v>
+        <v>701</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>836</v>
-      </c>
-      <c r="F9" s="19"/>
+        <v>702</v>
+      </c>
+      <c r="F9" s="15"/>
       <c r="G9" s="10" t="s">
-        <v>656</v>
+        <v>703</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>837</v>
-      </c>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
+        <v>704</v>
+      </c>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
     </row>
     <row r="10" customFormat="false" ht="50.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
-        <v>838</v>
+        <v>705</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>839</v>
-      </c>
-      <c r="C10" s="19"/>
+        <v>706</v>
+      </c>
+      <c r="C10" s="15"/>
       <c r="D10" s="10" t="s">
-        <v>840</v>
+        <v>707</v>
       </c>
       <c r="E10" s="10" t="s">
-        <v>841</v>
-      </c>
-      <c r="F10" s="19"/>
+        <v>708</v>
+      </c>
+      <c r="F10" s="15"/>
       <c r="G10" s="10" t="s">
-        <v>657</v>
+        <v>709</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>842</v>
-      </c>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
+        <v>710</v>
+      </c>
+      <c r="I10" s="15"/>
+      <c r="J10" s="15"/>
+      <c r="K10" s="15"/>
+      <c r="L10" s="15"/>
     </row>
     <row r="11" customFormat="false" ht="40.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
-        <v>843</v>
+        <v>711</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>844</v>
-      </c>
-      <c r="C11" s="19"/>
+        <v>712</v>
+      </c>
+      <c r="C11" s="15"/>
       <c r="D11" s="10" t="s">
-        <v>845</v>
+        <v>713</v>
       </c>
       <c r="E11" s="10" t="s">
-        <v>846</v>
-      </c>
-      <c r="F11" s="19"/>
+        <v>714</v>
+      </c>
+      <c r="F11" s="15"/>
       <c r="G11" s="10" t="s">
-        <v>658</v>
+        <v>715</v>
       </c>
       <c r="H11" s="10" t="s">
-        <v>847</v>
-      </c>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
+        <v>716</v>
+      </c>
+      <c r="I11" s="15"/>
+      <c r="J11" s="15"/>
+      <c r="K11" s="15"/>
+      <c r="L11" s="15"/>
     </row>
     <row r="12" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
-        <v>848</v>
+        <v>717</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>849</v>
-      </c>
-      <c r="C12" s="19"/>
+        <v>718</v>
+      </c>
+      <c r="C12" s="15"/>
       <c r="D12" s="10" t="s">
-        <v>850</v>
+        <v>719</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>851</v>
-      </c>
-      <c r="F12" s="19"/>
+        <v>720</v>
+      </c>
+      <c r="F12" s="15"/>
       <c r="G12" s="10" t="s">
-        <v>659</v>
+        <v>721</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>852</v>
-      </c>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
+        <v>722</v>
+      </c>
+      <c r="I12" s="15"/>
+      <c r="J12" s="15"/>
+      <c r="K12" s="15"/>
+      <c r="L12" s="15"/>
     </row>
     <row r="13" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
-        <v>853</v>
+        <v>723</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>854</v>
-      </c>
-      <c r="C13" s="19"/>
+        <v>724</v>
+      </c>
+      <c r="C13" s="15"/>
       <c r="D13" s="10" t="s">
-        <v>855</v>
+        <v>725</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>856</v>
-      </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="19"/>
-      <c r="H13" s="19"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="19"/>
-      <c r="K13" s="19"/>
-      <c r="L13" s="19"/>
+        <v>726</v>
+      </c>
+      <c r="F13" s="15"/>
+      <c r="G13" s="15"/>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15"/>
+      <c r="J13" s="15"/>
+      <c r="K13" s="15"/>
+      <c r="L13" s="15"/>
     </row>
     <row r="14" customFormat="false" ht="40.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
-        <v>857</v>
+        <v>727</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>858</v>
-      </c>
-      <c r="C14" s="19"/>
+        <v>728</v>
+      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="10" t="s">
-        <v>859</v>
+        <v>729</v>
       </c>
       <c r="E14" s="10" t="s">
-        <v>860</v>
-      </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="19"/>
-      <c r="H14" s="19"/>
-      <c r="I14" s="19"/>
-      <c r="J14" s="19"/>
-      <c r="K14" s="19"/>
-      <c r="L14" s="19"/>
+        <v>730</v>
+      </c>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="15"/>
+      <c r="K14" s="15"/>
+      <c r="L14" s="15"/>
     </row>
     <row r="15" customFormat="false" ht="30.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
-        <v>861</v>
+        <v>731</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>862</v>
-      </c>
-      <c r="C15" s="19"/>
+        <v>732</v>
+      </c>
+      <c r="C15" s="15"/>
       <c r="D15" s="10" t="s">
-        <v>863</v>
+        <v>733</v>
       </c>
       <c r="E15" s="10" t="s">
-        <v>864</v>
-      </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="19"/>
-      <c r="H15" s="19"/>
-      <c r="I15" s="19"/>
-      <c r="J15" s="19"/>
-      <c r="K15" s="19"/>
-      <c r="L15" s="19"/>
+        <v>734</v>
+      </c>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="15"/>
+      <c r="K15" s="15"/>
+      <c r="L15" s="15"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="19"/>
-      <c r="B16" s="19"/>
-      <c r="C16" s="19"/>
+      <c r="A16" s="15"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="15"/>
       <c r="D16" s="10" t="s">
-        <v>865</v>
+        <v>735</v>
       </c>
       <c r="E16" s="10" t="s">
-        <v>866</v>
-      </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="19"/>
-      <c r="H16" s="19"/>
-      <c r="I16" s="19"/>
-      <c r="J16" s="19"/>
-      <c r="K16" s="19"/>
-      <c r="L16" s="19"/>
+        <v>736</v>
+      </c>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15"/>
+      <c r="I16" s="15"/>
+      <c r="J16" s="15"/>
+      <c r="K16" s="15"/>
+      <c r="L16" s="15"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="19"/>
-      <c r="B17" s="19"/>
-      <c r="C17" s="19"/>
+      <c r="A17" s="15"/>
+      <c r="B17" s="15"/>
+      <c r="C17" s="15"/>
       <c r="D17" s="10" t="s">
-        <v>821</v>
+        <v>685</v>
       </c>
       <c r="E17" s="10" t="s">
-        <v>867</v>
-      </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="19"/>
-      <c r="H17" s="19"/>
-      <c r="I17" s="19"/>
-      <c r="J17" s="19"/>
-      <c r="K17" s="19"/>
-      <c r="L17" s="19"/>
+        <v>737</v>
+      </c>
+      <c r="F17" s="15"/>
+      <c r="G17" s="15"/>
+      <c r="H17" s="15"/>
+      <c r="I17" s="15"/>
+      <c r="J17" s="15"/>
+      <c r="K17" s="15"/>
+      <c r="L17" s="15"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D18" s="10" t="s">
-        <v>868</v>
+        <v>738</v>
       </c>
       <c r="E18" s="10" t="s">
-        <v>869</v>
+        <v>739</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D19" s="7" t="s">
-        <v>870</v>
+        <v>740</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>871</v>
+        <v>741</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D20" s="7" t="s">
-        <v>872</v>
+        <v>742</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>873</v>
+        <v>743</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D21" s="7" t="s">
-        <v>874</v>
+        <v>744</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>875</v>
+        <v>745</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="D22" s="7" t="s">
-        <v>876</v>
+        <v>746</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>877</v>
+        <v>747</v>
       </c>
     </row>
   </sheetData>
@@ -18305,4 +17157,2176 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:S73"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="11.52"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="20.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>749</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>750</v>
+      </c>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="1" t="s">
+        <v>751</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>691</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>697</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>703</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="O2" s="1"/>
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="s">
+        <v>752</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="1"/>
+      <c r="I3" s="1"/>
+      <c r="J3" s="1"/>
+      <c r="K3" s="1"/>
+      <c r="L3" s="1"/>
+      <c r="M3" s="1"/>
+      <c r="N3" s="1"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G4" s="3"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
+      <c r="K4" s="1"/>
+      <c r="L4" s="1"/>
+      <c r="M4" s="1"/>
+      <c r="N4" s="1"/>
+      <c r="O4" s="1"/>
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>757</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>754</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G5" s="3"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="s">
+        <v>758</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G6" s="3"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G7" s="3"/>
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>759</v>
+      </c>
+      <c r="D8" s="1"/>
+      <c r="E8" s="1"/>
+      <c r="F8" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G8" s="3"/>
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="s">
+        <v>762</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G9" s="3"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>764</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>763</v>
+      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="F10" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G10" s="3"/>
+      <c r="H10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>765</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>766</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G11" s="3"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>767</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>768</v>
+      </c>
+      <c r="D12" s="1"/>
+      <c r="E12" s="1"/>
+      <c r="F12" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G12" s="3"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>769</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>770</v>
+      </c>
+      <c r="D13" s="1"/>
+      <c r="E13" s="1"/>
+      <c r="F13" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G13" s="3"/>
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="17" t="s">
+        <v>771</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>772</v>
+      </c>
+      <c r="D14" s="1"/>
+      <c r="E14" s="1"/>
+      <c r="F14" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G14" s="3"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+      <c r="N14" s="1"/>
+      <c r="O14" s="1"/>
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>773</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>753</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>774</v>
+      </c>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+      <c r="F15" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G15" s="3"/>
+      <c r="H15" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I15" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
+      <c r="L15" s="1"/>
+      <c r="M15" s="1"/>
+      <c r="N15" s="1"/>
+      <c r="O15" s="1"/>
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1" t="s">
+        <v>775</v>
+      </c>
+      <c r="R15" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="89.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="s">
+        <v>776</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>777</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="R16" s="1"/>
+    </row>
+    <row r="17" customFormat="false" ht="59.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>780</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>781</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G17" s="3"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1"/>
+      <c r="M17" s="1"/>
+      <c r="N17" s="1"/>
+      <c r="O17" s="1"/>
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="59.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>782</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C18" s="18" t="s">
+        <v>781</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>776</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
+      <c r="L18" s="1"/>
+      <c r="M18" s="1"/>
+      <c r="N18" s="1"/>
+      <c r="O18" s="1"/>
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="118.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>783</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C19" s="18" t="s">
+        <v>784</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="E19" s="1"/>
+      <c r="F19" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
+      <c r="L19" s="1"/>
+      <c r="M19" s="1"/>
+      <c r="N19" s="1"/>
+      <c r="O19" s="1"/>
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>785</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>786</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="1"/>
+      <c r="F20" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="G20" s="3"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1"/>
+      <c r="P20" s="1"/>
+      <c r="Q20" s="19" t="s">
+        <v>787</v>
+      </c>
+      <c r="R20" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="19" t="s">
+        <v>788</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>789</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G21" s="3"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1"/>
+      <c r="P21" s="1"/>
+      <c r="R21" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="19" t="s">
+        <v>790</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>791</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>778</v>
+      </c>
+      <c r="E22" s="1"/>
+      <c r="F22" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G22" s="3"/>
+      <c r="H22" s="1"/>
+      <c r="I22" s="1"/>
+      <c r="J22" s="1"/>
+      <c r="K22" s="1"/>
+      <c r="L22" s="1"/>
+      <c r="M22" s="1"/>
+      <c r="N22" s="1"/>
+      <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="R22" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>792</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>793</v>
+      </c>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>794</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="0" t="s">
+        <v>795</v>
+      </c>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="s">
+        <v>796</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>799</v>
+      </c>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>800</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>801</v>
+      </c>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>803</v>
+      </c>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>804</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>805</v>
+      </c>
+      <c r="F29" s="2"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="s">
+        <v>806</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>807</v>
+      </c>
+      <c r="F30" s="2"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>808</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>809</v>
+      </c>
+      <c r="F31" s="2"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>811</v>
+      </c>
+      <c r="F32" s="2"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="F33" s="2"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="F34" s="2"/>
+      <c r="G34" s="3"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="137.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="18" t="s">
+        <v>817</v>
+      </c>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="3"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="F36" s="2"/>
+      <c r="G36" s="3"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>821</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>822</v>
+      </c>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="F37" s="2"/>
+      <c r="G37" s="3"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>824</v>
+      </c>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="3"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>825</v>
+      </c>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="3"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>826</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1" t="s">
+        <v>820</v>
+      </c>
+      <c r="F40" s="2"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>828</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>829</v>
+      </c>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1" t="s">
+        <v>823</v>
+      </c>
+      <c r="F41" s="2"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>830</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>831</v>
+      </c>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1" t="s">
+        <v>832</v>
+      </c>
+      <c r="F42" s="2"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>833</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C43" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1" t="s">
+        <v>835</v>
+      </c>
+      <c r="F43" s="2"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>836</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>837</v>
+      </c>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>838</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>839</v>
+      </c>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
+      <c r="K45" s="1"/>
+      <c r="L45" s="1"/>
+      <c r="M45" s="1"/>
+      <c r="N45" s="1"/>
+      <c r="O45" s="1"/>
+      <c r="P45" s="1"/>
+      <c r="Q45" s="1"/>
+      <c r="R45" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>840</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>841</v>
+      </c>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="3"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
+      <c r="K46" s="1"/>
+      <c r="L46" s="1"/>
+      <c r="M46" s="1"/>
+      <c r="N46" s="1"/>
+      <c r="O46" s="1"/>
+      <c r="P46" s="1"/>
+      <c r="Q46" s="1"/>
+      <c r="R46" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>842</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>843</v>
+      </c>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="3"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
+      <c r="K47" s="1"/>
+      <c r="L47" s="1"/>
+      <c r="M47" s="1"/>
+      <c r="N47" s="1"/>
+      <c r="O47" s="1"/>
+      <c r="P47" s="1"/>
+      <c r="Q47" s="1"/>
+      <c r="R47" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>844</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>845</v>
+      </c>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="3"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
+      <c r="K48" s="1"/>
+      <c r="L48" s="1"/>
+      <c r="M48" s="1"/>
+      <c r="N48" s="1"/>
+      <c r="O48" s="1"/>
+      <c r="P48" s="1"/>
+      <c r="Q48" s="1"/>
+      <c r="R48" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="1" t="s">
+        <v>846</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>847</v>
+      </c>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
+      <c r="K49" s="1"/>
+      <c r="L49" s="1"/>
+      <c r="M49" s="1"/>
+      <c r="N49" s="1"/>
+      <c r="O49" s="1"/>
+      <c r="P49" s="1"/>
+      <c r="Q49" s="1"/>
+      <c r="R49" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="69.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="1" t="s">
+        <v>848</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>849</v>
+      </c>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="1"/>
+      <c r="I50" s="1"/>
+      <c r="J50" s="1"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="1"/>
+      <c r="N50" s="1"/>
+      <c r="O50" s="1"/>
+      <c r="P50" s="1"/>
+      <c r="Q50" s="20" t="s">
+        <v>850</v>
+      </c>
+      <c r="R50" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="1" t="s">
+        <v>851</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>852</v>
+      </c>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="F51" s="2"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+      <c r="R51" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="D52" s="1"/>
+      <c r="E52" s="1" t="s">
+        <v>853</v>
+      </c>
+      <c r="F52" s="2"/>
+      <c r="G52" s="3"/>
+      <c r="H52" s="1"/>
+      <c r="I52" s="1"/>
+      <c r="J52" s="1"/>
+      <c r="K52" s="1"/>
+      <c r="L52" s="1"/>
+      <c r="M52" s="1"/>
+      <c r="N52" s="1"/>
+      <c r="O52" s="1"/>
+      <c r="P52" s="1"/>
+      <c r="Q52" s="1"/>
+      <c r="R52" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="2"/>
+      <c r="G53" s="3"/>
+      <c r="H53" s="1"/>
+      <c r="I53" s="1"/>
+      <c r="J53" s="1"/>
+      <c r="K53" s="1"/>
+      <c r="L53" s="1"/>
+      <c r="M53" s="1"/>
+      <c r="N53" s="1"/>
+      <c r="O53" s="1"/>
+      <c r="P53" s="1"/>
+      <c r="Q53" s="1"/>
+      <c r="R53" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="s">
+        <v>858</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="F54" s="2"/>
+      <c r="G54" s="3"/>
+      <c r="H54" s="1"/>
+      <c r="I54" s="1"/>
+      <c r="J54" s="1"/>
+      <c r="K54" s="1"/>
+      <c r="L54" s="1"/>
+      <c r="M54" s="1"/>
+      <c r="N54" s="1"/>
+      <c r="O54" s="1"/>
+      <c r="P54" s="1"/>
+      <c r="Q54" s="1"/>
+      <c r="R54" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="F55" s="2"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="1"/>
+      <c r="I55" s="1"/>
+      <c r="J55" s="1"/>
+      <c r="K55" s="1"/>
+      <c r="L55" s="1"/>
+      <c r="M55" s="1"/>
+      <c r="N55" s="1"/>
+      <c r="O55" s="1"/>
+      <c r="P55" s="1"/>
+      <c r="Q55" s="1"/>
+      <c r="R55" s="1" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1"/>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1"/>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+      <c r="F56" s="2"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="1"/>
+      <c r="I56" s="1"/>
+      <c r="J56" s="1"/>
+      <c r="K56" s="1"/>
+      <c r="L56" s="1"/>
+      <c r="M56" s="1"/>
+      <c r="N56" s="1"/>
+      <c r="O56" s="1"/>
+      <c r="P56" s="1"/>
+      <c r="Q56" s="1"/>
+      <c r="R56" s="1"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C57" s="1"/>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+      <c r="F57" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G57" s="3"/>
+      <c r="H57" s="1"/>
+      <c r="I57" s="1"/>
+      <c r="J57" s="1"/>
+      <c r="K57" s="1"/>
+      <c r="L57" s="1"/>
+      <c r="M57" s="1"/>
+      <c r="N57" s="1"/>
+      <c r="O57" s="1"/>
+      <c r="P57" s="1"/>
+      <c r="Q57" s="1"/>
+      <c r="R57" s="1"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C58" s="1"/>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+      <c r="F58" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G58" s="3"/>
+      <c r="H58" s="1"/>
+      <c r="I58" s="1"/>
+      <c r="J58" s="1"/>
+      <c r="K58" s="1"/>
+      <c r="L58" s="1"/>
+      <c r="M58" s="1"/>
+      <c r="N58" s="1"/>
+      <c r="O58" s="1"/>
+      <c r="P58" s="1"/>
+      <c r="Q58" s="1"/>
+      <c r="R58" s="1"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="B59" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C59" s="1"/>
+      <c r="D59" s="1"/>
+      <c r="E59" s="1"/>
+      <c r="F59" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G59" s="3"/>
+      <c r="H59" s="1"/>
+      <c r="I59" s="1"/>
+      <c r="J59" s="1"/>
+      <c r="K59" s="1"/>
+      <c r="L59" s="1"/>
+      <c r="M59" s="1"/>
+      <c r="N59" s="1"/>
+      <c r="O59" s="1"/>
+      <c r="P59" s="1"/>
+      <c r="Q59" s="1"/>
+      <c r="R59" s="1"/>
+    </row>
+    <row r="60" customFormat="false" ht="69.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="B60" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C60" s="18" t="s">
+        <v>866</v>
+      </c>
+      <c r="D60" s="1"/>
+      <c r="E60" s="1"/>
+      <c r="F60" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G60" s="3"/>
+      <c r="H60" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="I60" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="J60" s="1"/>
+      <c r="K60" s="1"/>
+      <c r="L60" s="1"/>
+      <c r="M60" s="1"/>
+      <c r="N60" s="1"/>
+      <c r="O60" s="1"/>
+      <c r="P60" s="1"/>
+      <c r="Q60" s="1"/>
+      <c r="R60" s="1"/>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="s">
+        <v>868</v>
+      </c>
+      <c r="B61" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="D61" s="1"/>
+      <c r="E61" s="1"/>
+      <c r="F61" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G61" s="3"/>
+      <c r="H61" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="I61" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="J61" s="1"/>
+      <c r="K61" s="1"/>
+      <c r="L61" s="1"/>
+      <c r="M61" s="1"/>
+      <c r="N61" s="1"/>
+      <c r="O61" s="1"/>
+      <c r="P61" s="1"/>
+      <c r="Q61" s="1"/>
+      <c r="R61" s="1"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="s">
+        <v>771</v>
+      </c>
+      <c r="B62" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C62" s="1"/>
+      <c r="D62" s="1"/>
+      <c r="E62" s="1"/>
+      <c r="F62" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G62" s="3"/>
+      <c r="H62" s="1"/>
+      <c r="I62" s="1"/>
+      <c r="J62" s="1"/>
+      <c r="K62" s="1"/>
+      <c r="L62" s="1"/>
+      <c r="M62" s="1"/>
+      <c r="N62" s="1"/>
+      <c r="O62" s="1"/>
+      <c r="P62" s="1"/>
+      <c r="Q62" s="1"/>
+      <c r="R62" s="1"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="D63" s="1"/>
+      <c r="E63" s="1"/>
+      <c r="F63" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G63" s="3"/>
+      <c r="H63" s="1" t="s">
+        <v>658</v>
+      </c>
+      <c r="I63" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="J63" s="1"/>
+      <c r="K63" s="1"/>
+      <c r="L63" s="1"/>
+      <c r="M63" s="1"/>
+      <c r="N63" s="1"/>
+      <c r="O63" s="1"/>
+      <c r="P63" s="1"/>
+      <c r="Q63" s="1"/>
+      <c r="R63" s="1"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="B64" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C64" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="D64" s="1"/>
+      <c r="E64" s="1"/>
+      <c r="F64" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G64" s="3"/>
+      <c r="H64" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="I64" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="J64" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="K64" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="L64" s="1" t="s">
+        <v>709</v>
+      </c>
+      <c r="M64" s="1" t="s">
+        <v>715</v>
+      </c>
+      <c r="N64" s="1" t="s">
+        <v>721</v>
+      </c>
+      <c r="O64" s="1"/>
+      <c r="P64" s="1"/>
+      <c r="Q64" s="1"/>
+      <c r="R64" s="1"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="B65" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C65" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="D65" s="1"/>
+      <c r="E65" s="1"/>
+      <c r="F65" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G65" s="3"/>
+      <c r="H65" s="1"/>
+      <c r="I65" s="1"/>
+      <c r="J65" s="1"/>
+      <c r="K65" s="1"/>
+      <c r="L65" s="1"/>
+      <c r="M65" s="1"/>
+      <c r="N65" s="1"/>
+      <c r="O65" s="1"/>
+      <c r="P65" s="1"/>
+      <c r="Q65" s="1"/>
+      <c r="R65" s="1"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="B66" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C66" s="1"/>
+      <c r="D66" s="1"/>
+      <c r="E66" s="1"/>
+      <c r="F66" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G66" s="3"/>
+      <c r="H66" s="1"/>
+      <c r="I66" s="1"/>
+      <c r="J66" s="1"/>
+      <c r="K66" s="1"/>
+      <c r="L66" s="1"/>
+      <c r="M66" s="1"/>
+      <c r="N66" s="1"/>
+      <c r="O66" s="1"/>
+      <c r="P66" s="1"/>
+      <c r="Q66" s="1"/>
+      <c r="R66" s="1"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="1" t="s">
+        <v>757</v>
+      </c>
+      <c r="B67" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C67" s="1"/>
+      <c r="D67" s="1"/>
+      <c r="E67" s="1"/>
+      <c r="F67" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G67" s="3"/>
+      <c r="H67" s="1"/>
+      <c r="I67" s="1"/>
+      <c r="J67" s="1"/>
+      <c r="K67" s="1"/>
+      <c r="L67" s="1"/>
+      <c r="M67" s="1"/>
+      <c r="N67" s="1"/>
+      <c r="O67" s="1"/>
+      <c r="P67" s="1"/>
+      <c r="Q67" s="1"/>
+      <c r="R67" s="1"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="1" t="s">
+        <v>760</v>
+      </c>
+      <c r="B68" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C68" s="1"/>
+      <c r="D68" s="1"/>
+      <c r="E68" s="1"/>
+      <c r="F68" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G68" s="3"/>
+      <c r="H68" s="1"/>
+      <c r="I68" s="1"/>
+      <c r="J68" s="1"/>
+      <c r="K68" s="1"/>
+      <c r="L68" s="1"/>
+      <c r="M68" s="1"/>
+      <c r="N68" s="1"/>
+      <c r="O68" s="1"/>
+      <c r="P68" s="1"/>
+      <c r="Q68" s="1"/>
+      <c r="R68" s="1"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="1" t="s">
+        <v>761</v>
+      </c>
+      <c r="B69" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="G69" s="3"/>
+      <c r="H69" s="1"/>
+      <c r="I69" s="1"/>
+      <c r="J69" s="1"/>
+      <c r="K69" s="1"/>
+      <c r="L69" s="1"/>
+      <c r="M69" s="1"/>
+      <c r="N69" s="1"/>
+      <c r="O69" s="1"/>
+      <c r="P69" s="1"/>
+      <c r="Q69" s="1"/>
+      <c r="R69" s="1"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="1" t="s">
+        <v>752</v>
+      </c>
+      <c r="B70" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G70" s="3"/>
+      <c r="H70" s="1"/>
+      <c r="I70" s="1"/>
+      <c r="J70" s="1"/>
+      <c r="K70" s="1"/>
+      <c r="L70" s="1"/>
+      <c r="M70" s="1"/>
+      <c r="N70" s="1"/>
+      <c r="O70" s="1"/>
+      <c r="P70" s="1"/>
+      <c r="Q70" s="1"/>
+      <c r="R70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="1" t="s">
+        <v>758</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G71" s="3"/>
+      <c r="H71" s="1"/>
+      <c r="I71" s="1"/>
+      <c r="J71" s="1"/>
+      <c r="K71" s="1"/>
+      <c r="L71" s="1"/>
+      <c r="M71" s="1"/>
+      <c r="N71" s="1"/>
+      <c r="O71" s="1"/>
+      <c r="P71" s="1"/>
+      <c r="Q71" s="1"/>
+      <c r="R71" s="1"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B72" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G72" s="3"/>
+      <c r="H72" s="1"/>
+      <c r="I72" s="1"/>
+      <c r="J72" s="1"/>
+      <c r="K72" s="1"/>
+      <c r="L72" s="1"/>
+      <c r="M72" s="1"/>
+      <c r="N72" s="1"/>
+      <c r="O72" s="1"/>
+      <c r="P72" s="1"/>
+      <c r="Q72" s="1"/>
+      <c r="R72" s="1"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="B73" s="1" t="s">
+        <v>273</v>
+      </c>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="2" t="s">
+        <v>779</v>
+      </c>
+      <c r="G73" s="3"/>
+      <c r="H73" s="1"/>
+      <c r="I73" s="1"/>
+      <c r="J73" s="1"/>
+      <c r="K73" s="1"/>
+      <c r="L73" s="1"/>
+      <c r="M73" s="1"/>
+      <c r="N73" s="1"/>
+      <c r="O73" s="1"/>
+      <c r="P73" s="1"/>
+      <c r="Q73" s="1"/>
+      <c r="R73" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regularna"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regularna"&amp;12Strona &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Uaktualniony diagram przepływu danych
</commit_message>
<xml_diff>
--- a/vignettes/definicje_zmiennych.xlsx
+++ b/vignettes/definicje_zmiennych.xlsx
@@ -3351,12 +3351,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -3433,9 +3433,9 @@
   <dimension ref="A1:AMH262"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A62" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A247" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="A274" activeCellId="0" sqref="A274"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22109,7 +22109,7 @@
   <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A274 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -22650,7 +22650,7 @@
   <dimension ref="A1:S73"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="topLeft" activeCell="I1" activeCellId="1" sqref="A274 I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -24910,7 +24910,7 @@
   <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L20" activeCellId="0" sqref="L20"/>
+      <selection pane="topLeft" activeCell="L20" activeCellId="1" sqref="A274 L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>